<commit_message>
fix float column for scrab standard
</commit_message>
<xml_diff>
--- a/apps/analysis/formats/QC_molds_daily_summary.xlsx
+++ b/apps/analysis/formats/QC_molds_daily_summary.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="1" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="daily" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="daily" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="27" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="28" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2" sheetId="4" state="visible" r:id="rId4"/>
@@ -15,13 +15,17 @@
     <sheet name="5" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="6" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="61" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="16" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="17" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="18" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="19" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
-    <externalReference r:id="rId12"/>
-    <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
+    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
     <definedName name="AccessDatabase" hidden="1">"C:\Documents and Settings\Administrator\My Documents\BITUNIL\FINANCE\SAMEER\Cost StudyHB.mdb"</definedName>
@@ -46,8 +50,9 @@
     <definedName name="Weight">[1]List!$K$4:$K$29</definedName>
     <definedName name="Year">'[4]Incom Statment'!#REF!</definedName>
     <definedName name="الاوزان">'[5]0'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'daily'!$A$2:$F$2</definedName>
   </definedNames>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1848,7 +1853,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -1856,7 +1861,7 @@
     <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
     <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
     <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="16.375" bestFit="1" customWidth="1" style="22" min="4" max="4"/>
+    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
     <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
     <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
   </cols>
@@ -2301,6 +2306,2510 @@
       <c r="B37" s="36" t="n"/>
       <c r="C37" s="4" t="n"/>
       <c r="D37" s="19" t="n"/>
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="9" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1" s="11">
+      <c r="A38" s="33" t="n"/>
+      <c r="B38" s="36" t="n"/>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="19" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1" s="11">
+      <c r="A39" s="33" t="n"/>
+      <c r="B39" s="36" t="n"/>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="19" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1" s="11">
+      <c r="A40" s="33" t="n"/>
+      <c r="B40" s="36" t="n"/>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="19" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" s="11">
+      <c r="A41" s="33" t="n"/>
+      <c r="B41" s="36" t="n"/>
+      <c r="C41" s="4" t="n"/>
+      <c r="D41" s="19" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+    </row>
+    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A42" s="34" t="n"/>
+      <c r="B42" s="37" t="n"/>
+      <c r="C42" s="5" t="n"/>
+      <c r="D42" s="20" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="10" t="n"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:F2">
+    <filterColumn colId="0" showButton="0"/>
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+    <filterColumn colId="4" showButton="0"/>
+  </autoFilter>
+  <mergeCells count="16">
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
+    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
+    <col width="25.875" customWidth="1" style="22" min="4" max="4"/>
+    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
+    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D1" s="17" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
+      <c r="A2" s="40" t="inlineStr">
+        <is>
+          <t>اولا : نسبة التالف على الماكينات</t>
+        </is>
+      </c>
+      <c r="B2" s="31" t="n"/>
+      <c r="C2" s="26" t="inlineStr">
+        <is>
+          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
+        </is>
+      </c>
+      <c r="D2" s="27" t="n"/>
+      <c r="E2" s="27" t="n"/>
+      <c r="F2" s="27" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
+        </is>
+      </c>
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D3" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.75" customHeight="1" s="11">
+      <c r="A4" s="41" t="n">
+        <v>1.185873605947955</v>
+      </c>
+      <c r="B4" s="42" t="n">
+        <v>1.369568950712691</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="19" t="inlineStr">
+        <is>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+    </row>
+    <row r="5" ht="21.75" customHeight="1" s="11">
+      <c r="A5" s="33" t="n"/>
+      <c r="B5" s="36" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="19" t="inlineStr">
+        <is>
+          <t>-قاعدة غسالة Lgo</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+    </row>
+    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B6" s="13" t="inlineStr">
+        <is>
+          <t>اعلي نسبة توالف</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="21.75" customHeight="1" s="11">
+      <c r="A7" s="14" t="n"/>
+      <c r="B7" s="16" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="19" t="inlineStr">
+        <is>
+          <t>LG43LM63-UM73</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+    </row>
+    <row r="8" ht="21.75" customHeight="1" s="11">
+      <c r="A8" s="14" t="n"/>
+      <c r="B8" s="15" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="19" t="inlineStr">
+        <is>
+          <t>70UQ80006LD</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
+      <c r="A9" s="12" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B9" s="13" t="inlineStr">
+        <is>
+          <t>وسيط التوالف</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="19" t="inlineStr">
+        <is>
+          <t>فوم  60*90 (دعامة و قاعدة)</t>
+        </is>
+      </c>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1" s="11">
+      <c r="A10" s="14" t="n"/>
+      <c r="B10" s="16" t="n"/>
+      <c r="C10" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" s="19" t="inlineStr">
+        <is>
+          <t>led32l2900</t>
+        </is>
+      </c>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A11" s="14" t="n"/>
+      <c r="B11" s="16" t="n"/>
+      <c r="C11" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" s="20" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
+        </is>
+      </c>
+      <c r="B12" s="31" t="n"/>
+      <c r="C12" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D12" s="29" t="n"/>
+      <c r="E12" s="29" t="n"/>
+      <c r="F12" s="29" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
+        </is>
+      </c>
+      <c r="B13" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D13" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="11">
+      <c r="A14" s="38" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="19" t="inlineStr">
+        <is>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="11">
+      <c r="A15" s="33" t="n"/>
+      <c r="B15" s="36" t="n"/>
+      <c r="C15" s="4" t="n"/>
+      <c r="D15" s="19" t="n"/>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="9" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1" s="11">
+      <c r="A16" s="33" t="n"/>
+      <c r="B16" s="36" t="n"/>
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="19" t="n"/>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="11">
+      <c r="A17" s="33" t="n"/>
+      <c r="B17" s="36" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="19" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1" s="11">
+      <c r="A18" s="33" t="n"/>
+      <c r="B18" s="36" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1" s="11">
+      <c r="A19" s="33" t="n"/>
+      <c r="B19" s="36" t="n"/>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="19" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1" s="11">
+      <c r="A20" s="33" t="n"/>
+      <c r="B20" s="36" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="19" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="11">
+      <c r="A21" s="33" t="n"/>
+      <c r="B21" s="36" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
+      <c r="A22" s="23" t="n"/>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="21" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+    </row>
+    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A23" s="30" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
+        </is>
+      </c>
+      <c r="B23" s="31" t="n"/>
+      <c r="C23" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D23" s="29" t="n"/>
+      <c r="E23" s="29" t="n"/>
+      <c r="F23" s="29" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A24" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B24" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D24" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="11">
+      <c r="A25" s="38" t="n">
+        <v>5</v>
+      </c>
+      <c r="B25" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" s="19" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="11">
+      <c r="A26" s="33" t="n"/>
+      <c r="B26" s="36" t="n"/>
+      <c r="C26" s="4" t="n"/>
+      <c r="D26" s="19" t="n"/>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="11">
+      <c r="A27" s="33" t="n"/>
+      <c r="B27" s="36" t="n"/>
+      <c r="C27" s="4" t="n"/>
+      <c r="D27" s="19" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1" s="11">
+      <c r="A28" s="33" t="n"/>
+      <c r="B28" s="36" t="n"/>
+      <c r="C28" s="4" t="n"/>
+      <c r="D28" s="19" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1" s="11">
+      <c r="A29" s="33" t="n"/>
+      <c r="B29" s="36" t="n"/>
+      <c r="C29" s="4" t="n"/>
+      <c r="D29" s="19" t="n"/>
+      <c r="E29" s="9" t="n"/>
+      <c r="F29" s="9" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1" s="11">
+      <c r="A30" s="33" t="n"/>
+      <c r="B30" s="36" t="n"/>
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="19" t="n"/>
+      <c r="E30" s="9" t="n"/>
+      <c r="F30" s="9" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1" s="11">
+      <c r="A31" s="33" t="n"/>
+      <c r="B31" s="36" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="19" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A32" s="33" t="n"/>
+      <c r="B32" s="36" t="n"/>
+      <c r="C32" s="5" t="n"/>
+      <c r="D32" s="20" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A33" s="30" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
+        </is>
+      </c>
+      <c r="B33" s="31" t="n"/>
+      <c r="C33" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D33" s="29" t="n"/>
+      <c r="E33" s="29" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A34" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D34" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1" s="11">
+      <c r="A35" s="32" t="n">
+        <v>5</v>
+      </c>
+      <c r="B35" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" s="19" t="inlineStr">
+        <is>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
+        </is>
+      </c>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1" s="11">
+      <c r="A36" s="33" t="n"/>
+      <c r="B36" s="36" t="n"/>
+      <c r="C36" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D36" s="19" t="inlineStr">
+        <is>
+          <t>led32l2900</t>
+        </is>
+      </c>
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="9" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1" s="11">
+      <c r="A37" s="33" t="n"/>
+      <c r="B37" s="36" t="n"/>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="19" t="n"/>
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="9" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1" s="11">
+      <c r="A38" s="33" t="n"/>
+      <c r="B38" s="36" t="n"/>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="19" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1" s="11">
+      <c r="A39" s="33" t="n"/>
+      <c r="B39" s="36" t="n"/>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="19" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1" s="11">
+      <c r="A40" s="33" t="n"/>
+      <c r="B40" s="36" t="n"/>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="19" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" s="11">
+      <c r="A41" s="33" t="n"/>
+      <c r="B41" s="36" t="n"/>
+      <c r="C41" s="4" t="n"/>
+      <c r="D41" s="19" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+    </row>
+    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A42" s="34" t="n"/>
+      <c r="B42" s="37" t="n"/>
+      <c r="C42" s="5" t="n"/>
+      <c r="D42" s="20" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="10" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
+    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
+    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
+    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D1" s="17" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
+      <c r="A2" s="40" t="inlineStr">
+        <is>
+          <t>اولا : نسبة التالف على الماكينات</t>
+        </is>
+      </c>
+      <c r="B2" s="31" t="n"/>
+      <c r="C2" s="26" t="inlineStr">
+        <is>
+          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
+        </is>
+      </c>
+      <c r="D2" s="27" t="n"/>
+      <c r="E2" s="27" t="n"/>
+      <c r="F2" s="27" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
+        </is>
+      </c>
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D3" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.75" customHeight="1" s="11">
+      <c r="A4" s="41" t="n">
+        <v>0.5631864548276853</v>
+      </c>
+      <c r="B4" s="42" t="n">
+        <v>0.5068482911971898</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="19" t="inlineStr">
+        <is>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+    </row>
+    <row r="5" ht="21.75" customHeight="1" s="11">
+      <c r="A5" s="33" t="n"/>
+      <c r="B5" s="36" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="19" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+    </row>
+    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B6" s="13" t="inlineStr">
+        <is>
+          <t>اعلي نسبة توالف</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>LG43LM63-UM73</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="21.75" customHeight="1" s="11">
+      <c r="A7" s="14" t="n"/>
+      <c r="B7" s="16" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="19" t="inlineStr">
+        <is>
+          <t>70UQ80006LD</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+    </row>
+    <row r="8" ht="21.75" customHeight="1" s="11">
+      <c r="A8" s="14" t="n"/>
+      <c r="B8" s="15" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="19" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
+      <c r="A9" s="12" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B9" s="13" t="inlineStr">
+        <is>
+          <t>وسيط التوالف</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="19" t="inlineStr">
+        <is>
+          <t>بوتجاز  90 تصدير</t>
+        </is>
+      </c>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1" s="11">
+      <c r="A10" s="14" t="n"/>
+      <c r="B10" s="16" t="n"/>
+      <c r="C10" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="19" t="inlineStr">
+        <is>
+          <t>فوم  60*90 (دعامة و قاعدة)</t>
+        </is>
+      </c>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A11" s="14" t="n"/>
+      <c r="B11" s="16" t="n"/>
+      <c r="C11" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" s="20" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
+        </is>
+      </c>
+      <c r="B12" s="31" t="n"/>
+      <c r="C12" s="28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D12" s="29" t="n"/>
+      <c r="E12" s="29" t="n"/>
+      <c r="F12" s="29" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
+        </is>
+      </c>
+      <c r="B13" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>48</v>
+      </c>
+      <c r="D13" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="11">
+      <c r="A14" s="38" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" s="39" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="19" t="inlineStr">
+        <is>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="11">
+      <c r="A15" s="33" t="n"/>
+      <c r="B15" s="36" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="D15" s="19" t="inlineStr">
+        <is>
+          <t>(إفتا)SAB</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="9" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1" s="11">
+      <c r="A16" s="33" t="n"/>
+      <c r="B16" s="36" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D16" s="19" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="11">
+      <c r="A17" s="33" t="n"/>
+      <c r="B17" s="36" t="n"/>
+      <c r="C17" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D17" s="19" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1" s="11">
+      <c r="A18" s="33" t="n"/>
+      <c r="B18" s="36" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1" s="11">
+      <c r="A19" s="33" t="n"/>
+      <c r="B19" s="36" t="n"/>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="19" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1" s="11">
+      <c r="A20" s="33" t="n"/>
+      <c r="B20" s="36" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="19" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="11">
+      <c r="A21" s="33" t="n"/>
+      <c r="B21" s="36" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
+      <c r="A22" s="23" t="n"/>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="21" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+    </row>
+    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A23" s="30" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
+        </is>
+      </c>
+      <c r="B23" s="31" t="n"/>
+      <c r="C23" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D23" s="29" t="n"/>
+      <c r="E23" s="29" t="n"/>
+      <c r="F23" s="29" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A24" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B24" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D24" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="11">
+      <c r="A25" s="38" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" s="19" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="11">
+      <c r="A26" s="33" t="n"/>
+      <c r="B26" s="36" t="n"/>
+      <c r="C26" s="4" t="n"/>
+      <c r="D26" s="19" t="n"/>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="11">
+      <c r="A27" s="33" t="n"/>
+      <c r="B27" s="36" t="n"/>
+      <c r="C27" s="4" t="n"/>
+      <c r="D27" s="19" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1" s="11">
+      <c r="A28" s="33" t="n"/>
+      <c r="B28" s="36" t="n"/>
+      <c r="C28" s="4" t="n"/>
+      <c r="D28" s="19" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1" s="11">
+      <c r="A29" s="33" t="n"/>
+      <c r="B29" s="36" t="n"/>
+      <c r="C29" s="4" t="n"/>
+      <c r="D29" s="19" t="n"/>
+      <c r="E29" s="9" t="n"/>
+      <c r="F29" s="9" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1" s="11">
+      <c r="A30" s="33" t="n"/>
+      <c r="B30" s="36" t="n"/>
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="19" t="n"/>
+      <c r="E30" s="9" t="n"/>
+      <c r="F30" s="9" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1" s="11">
+      <c r="A31" s="33" t="n"/>
+      <c r="B31" s="36" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="19" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A32" s="33" t="n"/>
+      <c r="B32" s="36" t="n"/>
+      <c r="C32" s="5" t="n"/>
+      <c r="D32" s="20" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A33" s="30" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
+        </is>
+      </c>
+      <c r="B33" s="31" t="n"/>
+      <c r="C33" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D33" s="29" t="n"/>
+      <c r="E33" s="29" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A34" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D34" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1" s="11">
+      <c r="A35" s="32" t="n">
+        <v>9</v>
+      </c>
+      <c r="B35" s="35" t="n"/>
+      <c r="C35" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="D35" s="19" t="inlineStr">
+        <is>
+          <t>(إفتا)SAB</t>
+        </is>
+      </c>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1" s="11">
+      <c r="A36" s="33" t="n"/>
+      <c r="B36" s="36" t="n"/>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="19" t="n"/>
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="9" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1" s="11">
+      <c r="A37" s="33" t="n"/>
+      <c r="B37" s="36" t="n"/>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="19" t="n"/>
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="9" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1" s="11">
+      <c r="A38" s="33" t="n"/>
+      <c r="B38" s="36" t="n"/>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="19" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1" s="11">
+      <c r="A39" s="33" t="n"/>
+      <c r="B39" s="36" t="n"/>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="19" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1" s="11">
+      <c r="A40" s="33" t="n"/>
+      <c r="B40" s="36" t="n"/>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="19" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" s="11">
+      <c r="A41" s="33" t="n"/>
+      <c r="B41" s="36" t="n"/>
+      <c r="C41" s="4" t="n"/>
+      <c r="D41" s="19" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+    </row>
+    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A42" s="34" t="n"/>
+      <c r="B42" s="37" t="n"/>
+      <c r="C42" s="5" t="n"/>
+      <c r="D42" s="20" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="10" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
+    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
+    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
+    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D1" s="17" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
+      <c r="A2" s="40" t="inlineStr">
+        <is>
+          <t>اولا : نسبة التالف على الماكينات</t>
+        </is>
+      </c>
+      <c r="B2" s="31" t="n"/>
+      <c r="C2" s="26" t="inlineStr">
+        <is>
+          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
+        </is>
+      </c>
+      <c r="D2" s="27" t="n"/>
+      <c r="E2" s="27" t="n"/>
+      <c r="F2" s="27" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
+        </is>
+      </c>
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D3" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.75" customHeight="1" s="11">
+      <c r="A4" s="41" t="n">
+        <v>0.7359661536647208</v>
+      </c>
+      <c r="B4" s="42" t="n">
+        <v>0.800203151205915</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="19" t="inlineStr">
+        <is>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+    </row>
+    <row r="5" ht="21.75" customHeight="1" s="11">
+      <c r="A5" s="33" t="n"/>
+      <c r="B5" s="36" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="19" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+    </row>
+    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B6" s="13" t="inlineStr">
+        <is>
+          <t>اعلي نسبة توالف</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>LG43LM63-UM73</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="21.75" customHeight="1" s="11">
+      <c r="A7" s="14" t="n"/>
+      <c r="B7" s="16" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="19" t="inlineStr">
+        <is>
+          <t>زانوسى العبد 305</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+    </row>
+    <row r="8" ht="21.75" customHeight="1" s="11">
+      <c r="A8" s="14" t="n"/>
+      <c r="B8" s="15" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="19" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
+      <c r="A9" s="12" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B9" s="13" t="inlineStr">
+        <is>
+          <t>وسيط التوالف</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="19" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1" s="11">
+      <c r="A10" s="14" t="n"/>
+      <c r="B10" s="16" t="n"/>
+      <c r="C10" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="19" t="inlineStr">
+        <is>
+          <t>بوتجاز  90 تصدير</t>
+        </is>
+      </c>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A11" s="14" t="n"/>
+      <c r="B11" s="16" t="n"/>
+      <c r="C11" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" s="20" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
+        </is>
+      </c>
+      <c r="B12" s="31" t="n"/>
+      <c r="C12" s="28" t="n">
+        <v>48</v>
+      </c>
+      <c r="D12" s="29" t="n"/>
+      <c r="E12" s="29" t="n"/>
+      <c r="F12" s="29" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
+        </is>
+      </c>
+      <c r="B13" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>49</v>
+      </c>
+      <c r="D13" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="11">
+      <c r="A14" s="38" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="19" t="inlineStr">
+        <is>
+          <t>زانوسى العبد 305</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="11">
+      <c r="A15" s="33" t="n"/>
+      <c r="B15" s="36" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D15" s="19" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="9" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1" s="11">
+      <c r="A16" s="33" t="n"/>
+      <c r="B16" s="36" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D16" s="19" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="11">
+      <c r="A17" s="33" t="n"/>
+      <c r="B17" s="36" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="19" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1" s="11">
+      <c r="A18" s="33" t="n"/>
+      <c r="B18" s="36" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1" s="11">
+      <c r="A19" s="33" t="n"/>
+      <c r="B19" s="36" t="n"/>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="19" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1" s="11">
+      <c r="A20" s="33" t="n"/>
+      <c r="B20" s="36" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="19" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="11">
+      <c r="A21" s="33" t="n"/>
+      <c r="B21" s="36" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
+      <c r="A22" s="23" t="n"/>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="21" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+    </row>
+    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A23" s="30" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
+        </is>
+      </c>
+      <c r="B23" s="31" t="n"/>
+      <c r="C23" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D23" s="29" t="n"/>
+      <c r="E23" s="29" t="n"/>
+      <c r="F23" s="29" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A24" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B24" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D24" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="11">
+      <c r="A25" s="38" t="n">
+        <v>8</v>
+      </c>
+      <c r="B25" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" s="19" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="11">
+      <c r="A26" s="33" t="n"/>
+      <c r="B26" s="36" t="n"/>
+      <c r="C26" s="4" t="n"/>
+      <c r="D26" s="19" t="n"/>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="11">
+      <c r="A27" s="33" t="n"/>
+      <c r="B27" s="36" t="n"/>
+      <c r="C27" s="4" t="n"/>
+      <c r="D27" s="19" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1" s="11">
+      <c r="A28" s="33" t="n"/>
+      <c r="B28" s="36" t="n"/>
+      <c r="C28" s="4" t="n"/>
+      <c r="D28" s="19" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1" s="11">
+      <c r="A29" s="33" t="n"/>
+      <c r="B29" s="36" t="n"/>
+      <c r="C29" s="4" t="n"/>
+      <c r="D29" s="19" t="n"/>
+      <c r="E29" s="9" t="n"/>
+      <c r="F29" s="9" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1" s="11">
+      <c r="A30" s="33" t="n"/>
+      <c r="B30" s="36" t="n"/>
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="19" t="n"/>
+      <c r="E30" s="9" t="n"/>
+      <c r="F30" s="9" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1" s="11">
+      <c r="A31" s="33" t="n"/>
+      <c r="B31" s="36" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="19" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A32" s="33" t="n"/>
+      <c r="B32" s="36" t="n"/>
+      <c r="C32" s="5" t="n"/>
+      <c r="D32" s="20" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A33" s="30" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
+        </is>
+      </c>
+      <c r="B33" s="31" t="n"/>
+      <c r="C33" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D33" s="29" t="n"/>
+      <c r="E33" s="29" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A34" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D34" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1" s="11">
+      <c r="A35" s="32" t="n">
+        <v>8</v>
+      </c>
+      <c r="B35" s="35" t="n"/>
+      <c r="C35" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" s="19" t="inlineStr">
+        <is>
+          <t>زانوسى العبد 305</t>
+        </is>
+      </c>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1" s="11">
+      <c r="A36" s="33" t="n"/>
+      <c r="B36" s="36" t="n"/>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="19" t="n"/>
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="9" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1" s="11">
+      <c r="A37" s="33" t="n"/>
+      <c r="B37" s="36" t="n"/>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="19" t="n"/>
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="9" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1" s="11">
+      <c r="A38" s="33" t="n"/>
+      <c r="B38" s="36" t="n"/>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="19" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1" s="11">
+      <c r="A39" s="33" t="n"/>
+      <c r="B39" s="36" t="n"/>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="19" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1" s="11">
+      <c r="A40" s="33" t="n"/>
+      <c r="B40" s="36" t="n"/>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="19" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" s="11">
+      <c r="A41" s="33" t="n"/>
+      <c r="B41" s="36" t="n"/>
+      <c r="C41" s="4" t="n"/>
+      <c r="D41" s="19" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+    </row>
+    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A42" s="34" t="n"/>
+      <c r="B42" s="37" t="n"/>
+      <c r="C42" s="5" t="n"/>
+      <c r="D42" s="20" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="10" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
+    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
+    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
+    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D1" s="17" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
+      <c r="A2" s="40" t="inlineStr">
+        <is>
+          <t>اولا : نسبة التالف على الماكينات</t>
+        </is>
+      </c>
+      <c r="B2" s="31" t="n"/>
+      <c r="C2" s="26" t="inlineStr">
+        <is>
+          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
+        </is>
+      </c>
+      <c r="D2" s="27" t="n"/>
+      <c r="E2" s="27" t="n"/>
+      <c r="F2" s="27" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
+        </is>
+      </c>
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D3" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.75" customHeight="1" s="11">
+      <c r="A4" s="41" t="n">
+        <v>0.9133815905311553</v>
+      </c>
+      <c r="B4" s="42" t="n">
+        <v>0.9587705450831091</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="inlineStr">
+        <is>
+          <t>زانوسى العبد 305</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+    </row>
+    <row r="5" ht="21.75" customHeight="1" s="11">
+      <c r="A5" s="33" t="n"/>
+      <c r="B5" s="36" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="19" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+    </row>
+    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B6" s="13" t="inlineStr">
+        <is>
+          <t>اعلي نسبة توالف</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="21.75" customHeight="1" s="11">
+      <c r="A7" s="14" t="n"/>
+      <c r="B7" s="16" t="n"/>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="19" t="n"/>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+    </row>
+    <row r="8" ht="21.75" customHeight="1" s="11">
+      <c r="A8" s="14" t="n"/>
+      <c r="B8" s="15" t="n"/>
+      <c r="C8" s="4" t="n"/>
+      <c r="D8" s="19" t="n"/>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
+      <c r="A9" s="12" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B9" s="13" t="inlineStr">
+        <is>
+          <t>وسيط التوالف</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n"/>
+      <c r="D9" s="19" t="n"/>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1" s="11">
+      <c r="A10" s="14" t="n"/>
+      <c r="B10" s="16" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="19" t="n"/>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A11" s="14" t="n"/>
+      <c r="B11" s="16" t="n"/>
+      <c r="C11" s="5" t="n"/>
+      <c r="D11" s="20" t="n"/>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
+        </is>
+      </c>
+      <c r="B12" s="31" t="n"/>
+      <c r="C12" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D12" s="29" t="n"/>
+      <c r="E12" s="29" t="n"/>
+      <c r="F12" s="29" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
+        </is>
+      </c>
+      <c r="B13" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D13" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="11">
+      <c r="A14" s="38" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" s="39" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="19" t="inlineStr">
+        <is>
+          <t>زانوسى العبد 305</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="11">
+      <c r="A15" s="33" t="n"/>
+      <c r="B15" s="36" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D15" s="19" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="9" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1" s="11">
+      <c r="A16" s="33" t="n"/>
+      <c r="B16" s="36" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D16" s="19" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="11">
+      <c r="A17" s="33" t="n"/>
+      <c r="B17" s="36" t="n"/>
+      <c r="C17" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D17" s="19" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1" s="11">
+      <c r="A18" s="33" t="n"/>
+      <c r="B18" s="36" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1" s="11">
+      <c r="A19" s="33" t="n"/>
+      <c r="B19" s="36" t="n"/>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="19" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1" s="11">
+      <c r="A20" s="33" t="n"/>
+      <c r="B20" s="36" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="19" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="11">
+      <c r="A21" s="33" t="n"/>
+      <c r="B21" s="36" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
+      <c r="A22" s="23" t="n"/>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="21" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+    </row>
+    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A23" s="30" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
+        </is>
+      </c>
+      <c r="B23" s="31" t="n"/>
+      <c r="C23" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D23" s="29" t="n"/>
+      <c r="E23" s="29" t="n"/>
+      <c r="F23" s="29" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A24" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B24" s="13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D24" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="11">
+      <c r="A25" s="38" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" s="19" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="11">
+      <c r="A26" s="33" t="n"/>
+      <c r="B26" s="36" t="n"/>
+      <c r="C26" s="4" t="n"/>
+      <c r="D26" s="19" t="n"/>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="11">
+      <c r="A27" s="33" t="n"/>
+      <c r="B27" s="36" t="n"/>
+      <c r="C27" s="4" t="n"/>
+      <c r="D27" s="19" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1" s="11">
+      <c r="A28" s="33" t="n"/>
+      <c r="B28" s="36" t="n"/>
+      <c r="C28" s="4" t="n"/>
+      <c r="D28" s="19" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1" s="11">
+      <c r="A29" s="33" t="n"/>
+      <c r="B29" s="36" t="n"/>
+      <c r="C29" s="4" t="n"/>
+      <c r="D29" s="19" t="n"/>
+      <c r="E29" s="9" t="n"/>
+      <c r="F29" s="9" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1" s="11">
+      <c r="A30" s="33" t="n"/>
+      <c r="B30" s="36" t="n"/>
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="19" t="n"/>
+      <c r="E30" s="9" t="n"/>
+      <c r="F30" s="9" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1" s="11">
+      <c r="A31" s="33" t="n"/>
+      <c r="B31" s="36" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="19" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A32" s="33" t="n"/>
+      <c r="B32" s="36" t="n"/>
+      <c r="C32" s="5" t="n"/>
+      <c r="D32" s="20" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
+      <c r="A33" s="30" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
+        </is>
+      </c>
+      <c r="B33" s="31" t="n"/>
+      <c r="C33" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D33" s="29" t="n"/>
+      <c r="E33" s="29" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
+      <c r="A34" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D34" s="18" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1" s="11">
+      <c r="A35" s="32" t="n">
+        <v>9</v>
+      </c>
+      <c r="B35" s="35" t="n"/>
+      <c r="C35" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" s="19" t="inlineStr">
+        <is>
+          <t>زانوسى العبد 305</t>
+        </is>
+      </c>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1" s="11">
+      <c r="A36" s="33" t="n"/>
+      <c r="B36" s="36" t="n"/>
+      <c r="C36" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D36" s="19" t="inlineStr">
+        <is>
+          <t>LG65UP81</t>
+        </is>
+      </c>
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="9" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1" s="11">
+      <c r="A37" s="33" t="n"/>
+      <c r="B37" s="36" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="D37" s="19" t="inlineStr">
+        <is>
+          <t>جزء وسط E554</t>
+        </is>
+      </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
@@ -2377,7 +4886,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView rightToLeft="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A42"/>
+      <selection activeCell="B35" sqref="B35:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -5431,7 +7940,7 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="F42" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding more email obtion for followup
</commit_message>
<xml_diff>
--- a/apps/analysis/formats/QC_molds_daily_summary.xlsx
+++ b/apps/analysis/formats/QC_molds_daily_summary.xlsx
@@ -3,25 +3,22 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="1" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="1" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="29" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="4" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="8" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="9" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="6" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="1" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="11" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="16" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="17" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="18" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
-    <externalReference r:id="rId12"/>
-    <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="AccessDatabase" hidden="1">"C:\Documents and Settings\Administrator\My Documents\BITUNIL\FINANCE\SAMEER\Cost StudyHB.mdb"</definedName>
@@ -48,7 +45,7 @@
     <definedName name="الاوزان">'[5]0'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'daily'!$A$2:$F$2</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -2355,8 +2352,8 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F42"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F42" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -2377,11 +2374,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D1" s="17" t="n">
         <v>2022</v>
@@ -2439,17 +2436,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1" s="11">
       <c r="A4" s="39" t="n">
-        <v>1.461701521814788</v>
+        <v>0.7635200386286818</v>
       </c>
       <c r="B4" s="40" t="n">
-        <v>1.896463352127114</v>
+        <v>0.7398501803384815</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="19" t="inlineStr">
         <is>
-          <t>فوم صندوق سمك التابوت</t>
+          <t>فوم طقم رويال جاز المعدل</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -2459,11 +2456,11 @@
       <c r="A5" s="31" t="n"/>
       <c r="B5" s="34" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="19" t="inlineStr">
         <is>
-          <t>صندوق سمك 5ك بنى سويف</t>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -2481,11 +2478,11 @@
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" s="19" t="inlineStr">
         <is>
-          <t>صندوق 10 ك فلات</t>
+          <t>LG75UP77-front</t>
         </is>
       </c>
       <c r="E6" s="9" t="n"/>
@@ -2495,11 +2492,11 @@
       <c r="A7" s="14" t="n"/>
       <c r="B7" s="16" t="n"/>
       <c r="C7" s="4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7" s="19" t="inlineStr">
         <is>
-          <t>LG43LM63-UM73</t>
+          <t>زانوسى العبد 305</t>
         </is>
       </c>
       <c r="E7" s="9" t="n"/>
@@ -2509,11 +2506,11 @@
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="15" t="n"/>
       <c r="C8" s="4" t="n">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="D8" s="19" t="inlineStr">
         <is>
-          <t>LG65UM73</t>
+          <t>جانب حماية يمين / شمال</t>
         </is>
       </c>
       <c r="E8" s="9" t="n"/>
@@ -2530,28 +2527,16 @@
           <t>وسيط التوالف</t>
         </is>
       </c>
-      <c r="C9" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D9" s="19" t="inlineStr">
-        <is>
-          <t>فوم طقم رويال جاز المعدل</t>
-        </is>
-      </c>
+      <c r="C9" s="4" t="n"/>
+      <c r="D9" s="19" t="n"/>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
     <row r="10" ht="18" customHeight="1" s="11">
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="16" t="n"/>
-      <c r="C10" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D10" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="19" t="n"/>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
     </row>
@@ -2613,17 +2598,17 @@
     </row>
     <row r="14" ht="18" customHeight="1" s="11">
       <c r="A14" s="36" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" s="37" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="19" t="inlineStr">
         <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
+          <t>oled55cs6la</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -2633,11 +2618,11 @@
       <c r="A15" s="31" t="n"/>
       <c r="B15" s="34" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D15" s="19" t="inlineStr">
         <is>
-          <t>صندوق سمك 25 ك</t>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -2647,11 +2632,11 @@
       <c r="A16" s="31" t="n"/>
       <c r="B16" s="34" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D16" s="19" t="inlineStr">
         <is>
-          <t>فوم صندوق سمك التابوت</t>
+          <t>زانوسى العبد 305</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
@@ -2661,11 +2646,11 @@
       <c r="A17" s="31" t="n"/>
       <c r="B17" s="34" t="n"/>
       <c r="C17" s="4" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="D17" s="19" t="inlineStr">
         <is>
-          <t>صندوق سمك 5ك بنى سويف</t>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
         </is>
       </c>
       <c r="E17" s="9" t="n"/>
@@ -2675,11 +2660,11 @@
       <c r="A18" s="31" t="n"/>
       <c r="B18" s="34" t="n"/>
       <c r="C18" s="4" t="n">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D18" s="19" t="inlineStr">
         <is>
-          <t>(إفتا)SAB</t>
+          <t>فوم قاعده 60*60</t>
         </is>
       </c>
       <c r="E18" s="9" t="n"/>
@@ -2688,56 +2673,32 @@
     <row r="19" ht="18" customHeight="1" s="11">
       <c r="A19" s="31" t="n"/>
       <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="D19" s="19" t="inlineStr">
-        <is>
-          <t>Stop Coller S4</t>
-        </is>
-      </c>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="19" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
     <row r="20" ht="18" customHeight="1" s="11">
       <c r="A20" s="31" t="n"/>
       <c r="B20" s="34" t="n"/>
-      <c r="C20" s="4" t="n">
-        <v>46</v>
-      </c>
-      <c r="D20" s="19" t="inlineStr">
-        <is>
-          <t>جانب حماية يمين / شمال</t>
-        </is>
-      </c>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="19" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
     <row r="21" ht="18" customHeight="1" s="11">
       <c r="A21" s="31" t="n"/>
       <c r="B21" s="34" t="n"/>
-      <c r="C21" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D21" s="19" t="inlineStr">
-        <is>
-          <t>فوم طقم رويال جاز المعدل</t>
-        </is>
-      </c>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="19" t="n"/>
       <c r="E21" s="9" t="n"/>
       <c r="F21" s="9" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
       <c r="A22" s="23" t="n"/>
       <c r="B22" s="9" t="n"/>
-      <c r="C22" s="6" t="n">
-        <v>48</v>
-      </c>
-      <c r="D22" s="21" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="21" t="n"/>
       <c r="E22" s="9" t="n"/>
       <c r="F22" s="9" t="n"/>
     </row>
@@ -2748,8 +2709,10 @@
         </is>
       </c>
       <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="n">
-        <v>49</v>
+      <c r="C23" s="26" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
       </c>
       <c r="D23" s="27" t="n"/>
       <c r="E23" s="27" t="n"/>
@@ -2789,10 +2752,10 @@
     </row>
     <row r="25" ht="18" customHeight="1" s="11">
       <c r="A25" s="36" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B25" s="37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="19" t="n"/>
@@ -2904,15 +2867,17 @@
     </row>
     <row r="35" ht="18" customHeight="1" s="11">
       <c r="A35" s="30" t="n">
-        <v>18</v>
-      </c>
-      <c r="B35" s="33" t="n"/>
+        <v>13</v>
+      </c>
+      <c r="B35" s="33" t="n">
+        <v>3</v>
+      </c>
       <c r="C35" s="4" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D35" s="19" t="inlineStr">
         <is>
-          <t>فوم حمايةالعداد2</t>
+          <t>LG43LM63-UM73</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -2921,16 +2886,28 @@
     <row r="36" ht="18" customHeight="1" s="11">
       <c r="A36" s="31" t="n"/>
       <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n"/>
-      <c r="D36" s="19" t="n"/>
+      <c r="C36" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D36" s="19" t="inlineStr">
+        <is>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
+        </is>
+      </c>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1" s="11">
       <c r="A37" s="31" t="n"/>
       <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="19" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D37" s="19" t="inlineStr">
+        <is>
+          <t>زانوسى العبد 305</t>
+        </is>
+      </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
@@ -3028,11 +3005,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="17" t="n">
         <v>2022</v>
@@ -3090,17 +3067,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1" s="11">
       <c r="A4" s="39" t="n">
-        <v>1.273046532045654</v>
+        <v>0.7839313572542903</v>
       </c>
       <c r="B4" s="40" t="n">
-        <v>1.298470295268588</v>
+        <v>0.7853403141361256</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D4" s="19" t="inlineStr">
         <is>
-          <t>LG65UP77_TB</t>
+          <t>70UQ80006LD</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -3109,14 +3086,8 @@
     <row r="5" ht="21.75" customHeight="1" s="11">
       <c r="A5" s="31" t="n"/>
       <c r="B5" s="34" t="n"/>
-      <c r="C5" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" s="19" t="inlineStr">
-        <is>
-          <t>LG Nano80</t>
-        </is>
-      </c>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="19" t="n"/>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
@@ -3131,28 +3102,16 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>(إفتا)SAB</t>
-        </is>
-      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="19" t="n"/>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1" s="11">
       <c r="A7" s="14" t="n"/>
       <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D7" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
-        </is>
-      </c>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="19" t="n"/>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
@@ -3249,14 +3208,14 @@
         <v>10</v>
       </c>
       <c r="B14" s="37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="19" t="inlineStr">
         <is>
-          <t>صندوق سمك 25 ك</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -3266,11 +3225,11 @@
       <c r="A15" s="31" t="n"/>
       <c r="B15" s="34" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="19" t="inlineStr">
         <is>
-          <t>فوم صندوق سمك 35 ك</t>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -3280,11 +3239,11 @@
       <c r="A16" s="31" t="n"/>
       <c r="B16" s="34" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D16" s="19" t="inlineStr">
         <is>
-          <t>OLED65cs6la</t>
+          <t>LG43UP79</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
@@ -3308,11 +3267,11 @@
       <c r="A18" s="31" t="n"/>
       <c r="B18" s="34" t="n"/>
       <c r="C18" s="4" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="19" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
         </is>
       </c>
       <c r="E18" s="9" t="n"/>
@@ -3321,14 +3280,8 @@
     <row r="19" ht="18" customHeight="1" s="11">
       <c r="A19" s="31" t="n"/>
       <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D19" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="19" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
@@ -3405,20 +3358,12 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n">
-        <v>10</v>
-      </c>
+      <c r="A25" s="36" t="n"/>
       <c r="B25" s="37" t="n">
-        <v>6</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D25" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="n"/>
+      <c r="D25" s="19" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -3527,15 +3472,17 @@
     </row>
     <row r="35" ht="18" customHeight="1" s="11">
       <c r="A35" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="B35" s="33" t="n"/>
+        <v>14</v>
+      </c>
+      <c r="B35" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="C35" s="4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D35" s="19" t="inlineStr">
         <is>
-          <t>OLED65cs6la</t>
+          <t>زانوسى العبد 305</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -3544,56 +3491,32 @@
     <row r="36" ht="18" customHeight="1" s="11">
       <c r="A36" s="31" t="n"/>
       <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D36" s="19" t="inlineStr">
-        <is>
-          <t>ايس كريم البرنس</t>
-        </is>
-      </c>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="19" t="n"/>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1" s="11">
       <c r="A37" s="31" t="n"/>
       <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D37" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="19" t="n"/>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1" s="11">
       <c r="A38" s="31" t="n"/>
       <c r="B38" s="34" t="n"/>
-      <c r="C38" s="4" t="n">
-        <v>26</v>
-      </c>
-      <c r="D38" s="19" t="inlineStr">
-        <is>
-          <t>فوم حمايةالعداد2</t>
-        </is>
-      </c>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="19" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
     <row r="39" ht="18" customHeight="1" s="11">
       <c r="A39" s="31" t="n"/>
       <c r="B39" s="34" t="n"/>
-      <c r="C39" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D39" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
-        </is>
-      </c>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="19" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
@@ -3675,11 +3598,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="17" t="n">
         <v>2022</v>
@@ -3737,13 +3660,13 @@
     </row>
     <row r="4" ht="21.75" customHeight="1" s="11">
       <c r="A4" s="39" t="n">
-        <v>2.464087919695396</v>
+        <v>0.8631486308093288</v>
       </c>
       <c r="B4" s="40" t="n">
-        <v>2.903884215734785</v>
+        <v>0.8631207917212707</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="19" t="inlineStr">
         <is>
@@ -3757,11 +3680,11 @@
       <c r="A5" s="31" t="n"/>
       <c r="B5" s="34" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5" s="19" t="inlineStr">
         <is>
-          <t>غطاء صندوق سمك 20 ك فلات الجديدة</t>
+          <t>LG43UP79</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -3779,11 +3702,11 @@
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D6" s="19" t="inlineStr">
         <is>
-          <t>فوم  60*90 (دعامة و قاعدة)</t>
+          <t>70UQ80006LD</t>
         </is>
       </c>
       <c r="E6" s="9" t="n"/>
@@ -3793,11 +3716,11 @@
       <c r="A7" s="14" t="n"/>
       <c r="B7" s="16" t="n"/>
       <c r="C7" s="4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D7" s="19" t="inlineStr">
         <is>
-          <t>LG75UP77set</t>
+          <t>زانوسي العبد 303-304-308-314</t>
         </is>
       </c>
       <c r="E7" s="9" t="n"/>
@@ -3806,14 +3729,8 @@
     <row r="8" ht="21.75" customHeight="1" s="11">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D8" s="19" t="inlineStr">
-        <is>
-          <t>صندوق 10 ك فلات</t>
-        </is>
-      </c>
+      <c r="C8" s="4" t="n"/>
+      <c r="D8" s="19" t="n"/>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -3828,42 +3745,24 @@
           <t>وسيط التوالف</t>
         </is>
       </c>
-      <c r="C9" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D9" s="19" t="inlineStr">
-        <is>
-          <t>LG32LM55-LM63</t>
-        </is>
-      </c>
+      <c r="C9" s="4" t="n"/>
+      <c r="D9" s="19" t="n"/>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
     <row r="10" ht="18" customHeight="1" s="11">
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="16" t="n"/>
-      <c r="C10" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D10" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="19" t="n"/>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
     </row>
     <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
       <c r="A11" s="14" t="n"/>
       <c r="B11" s="16" t="n"/>
-      <c r="C11" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="D11" s="20" t="inlineStr">
-        <is>
-          <t>فوم طقم رويال جاز المعدل</t>
-        </is>
-      </c>
+      <c r="C11" s="5" t="n"/>
+      <c r="D11" s="20" t="n"/>
       <c r="E11" s="9" t="n"/>
       <c r="F11" s="9" t="n"/>
     </row>
@@ -3917,17 +3816,17 @@
     </row>
     <row r="14" ht="18" customHeight="1" s="11">
       <c r="A14" s="36" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" s="37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D14" s="19" t="inlineStr">
         <is>
-          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -3937,11 +3836,11 @@
       <c r="A15" s="31" t="n"/>
       <c r="B15" s="34" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D15" s="19" t="inlineStr">
         <is>
-          <t>زانوسى العبد 305</t>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -3951,11 +3850,11 @@
       <c r="A16" s="31" t="n"/>
       <c r="B16" s="34" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D16" s="19" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>LG43UP79</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
@@ -3965,11 +3864,11 @@
       <c r="A17" s="31" t="n"/>
       <c r="B17" s="34" t="n"/>
       <c r="C17" s="4" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D17" s="19" t="inlineStr">
         <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
+          <t>زانوسى العبد 305</t>
         </is>
       </c>
       <c r="E17" s="9" t="n"/>
@@ -3978,8 +3877,14 @@
     <row r="18" ht="18" customHeight="1" s="11">
       <c r="A18" s="31" t="n"/>
       <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="19" t="n"/>
+      <c r="C18" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D18" s="19" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
@@ -4064,20 +3969,12 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n">
-        <v>10</v>
-      </c>
+      <c r="A25" s="36" t="n"/>
       <c r="B25" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D25" s="19" t="inlineStr">
-        <is>
-          <t>tosh 43</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="n"/>
+      <c r="D25" s="19" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -4186,15 +4083,17 @@
     </row>
     <row r="35" ht="18" customHeight="1" s="11">
       <c r="A35" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="B35" s="33" t="n"/>
+        <v>15</v>
+      </c>
+      <c r="B35" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="C35" s="4" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D35" s="19" t="inlineStr">
         <is>
-          <t>فوم  60*90 (دعامة و قاعدة)</t>
+          <t>زانوسى العبد 305</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -4203,14 +4102,8 @@
     <row r="36" ht="18" customHeight="1" s="11">
       <c r="A36" s="31" t="n"/>
       <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D36" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="19" t="n"/>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
@@ -4316,11 +4209,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="17" t="n">
         <v>2022</v>
@@ -4378,17 +4271,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1" s="11">
       <c r="A4" s="39" t="n">
-        <v>1.00207468879668</v>
+        <v>0.7745091378490386</v>
       </c>
       <c r="B4" s="40" t="n">
-        <v>0.9149712516585582</v>
+        <v>0.6802721088435374</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D4" s="19" t="inlineStr">
         <is>
-          <t>LG65UM73</t>
+          <t>فوم طقم سخان غاز 10 لتر</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -4398,11 +4291,11 @@
       <c r="A5" s="31" t="n"/>
       <c r="B5" s="34" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="D5" s="19" t="inlineStr">
         <is>
-          <t>LG Nano80</t>
+          <t>فوم قاعده 60*60</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -4419,42 +4312,24 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>LG75UP77set</t>
-        </is>
-      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="19" t="n"/>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1" s="11">
       <c r="A7" s="14" t="n"/>
       <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D7" s="19" t="inlineStr">
-        <is>
-          <t>tosh 43</t>
-        </is>
-      </c>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="19" t="n"/>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1" s="11">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D8" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
-        </is>
-      </c>
+      <c r="C8" s="4" t="n"/>
+      <c r="D8" s="19" t="n"/>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -4540,17 +4415,17 @@
     </row>
     <row r="14" ht="18" customHeight="1" s="11">
       <c r="A14" s="36" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" s="37" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="19" t="inlineStr">
         <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
+          <t>oled55cs6la</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -4564,7 +4439,7 @@
       </c>
       <c r="D15" s="19" t="inlineStr">
         <is>
-          <t>ايس كريم كينج</t>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -4574,11 +4449,11 @@
       <c r="A16" s="31" t="n"/>
       <c r="B16" s="34" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="D16" s="19" t="inlineStr">
         <is>
-          <t>زانوسى العبد 305</t>
+          <t>زانوسي 70 سم -2 (قاعدة ، كفر)</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
@@ -4588,11 +4463,11 @@
       <c r="A17" s="31" t="n"/>
       <c r="B17" s="34" t="n"/>
       <c r="C17" s="4" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" s="19" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
         </is>
       </c>
       <c r="E17" s="9" t="n"/>
@@ -4601,28 +4476,16 @@
     <row r="18" ht="18" customHeight="1" s="11">
       <c r="A18" s="31" t="n"/>
       <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D18" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="19" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1" s="11">
       <c r="A19" s="31" t="n"/>
       <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D19" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
-        </is>
-      </c>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="19" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
@@ -4700,19 +4563,11 @@
     </row>
     <row r="25" ht="18" customHeight="1" s="11">
       <c r="A25" s="36" t="n">
-        <v>12</v>
-      </c>
-      <c r="B25" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D25" s="19" t="inlineStr">
-        <is>
-          <t>LG75UP77set</t>
-        </is>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B25" s="37" t="n"/>
+      <c r="C25" s="4" t="n"/>
+      <c r="D25" s="19" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -4821,15 +4676,17 @@
     </row>
     <row r="35" ht="18" customHeight="1" s="11">
       <c r="A35" s="30" t="n">
-        <v>12</v>
-      </c>
-      <c r="B35" s="33" t="n"/>
+        <v>11</v>
+      </c>
+      <c r="B35" s="33" t="n">
+        <v>4</v>
+      </c>
       <c r="C35" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="19" t="inlineStr">
         <is>
-          <t>فوم  60*90 (دعامة و قاعدة)</t>
+          <t>LG43LM63-UM73</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -4839,11 +4696,11 @@
       <c r="A36" s="31" t="n"/>
       <c r="B36" s="34" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D36" s="19" t="inlineStr">
         <is>
-          <t>زانوسى العبد 305</t>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
@@ -4852,16 +4709,28 @@
     <row r="37" ht="18" customHeight="1" s="11">
       <c r="A37" s="31" t="n"/>
       <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="19" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D37" s="19" t="inlineStr">
+        <is>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
+        </is>
+      </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1" s="11">
       <c r="A38" s="31" t="n"/>
       <c r="B38" s="34" t="n"/>
-      <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
+      <c r="C38" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="D38" s="19" t="inlineStr">
+        <is>
+          <t>فوم طقم سخان غاز 10 لتر</t>
+        </is>
+      </c>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
@@ -4951,11 +4820,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D1" s="17" t="n">
         <v>2022</v>
@@ -5013,33 +4882,21 @@
     </row>
     <row r="4" ht="21.75" customHeight="1" s="11">
       <c r="A4" s="39" t="n">
-        <v>0.5309307376719492</v>
+        <v>101.010101010101</v>
       </c>
       <c r="B4" s="40" t="n">
-        <v>0.6155412597769241</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>LG65UM73</t>
-        </is>
-      </c>
+        <v>101.2345679012346</v>
+      </c>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="19" t="n"/>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
     </row>
     <row r="5" ht="21.75" customHeight="1" s="11">
       <c r="A5" s="31" t="n"/>
       <c r="B5" s="34" t="n"/>
-      <c r="C5" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="19" t="inlineStr">
-        <is>
-          <t>FRONT 43LM63</t>
-        </is>
-      </c>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="19" t="n"/>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
@@ -5054,42 +4911,24 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>LG Nano80</t>
-        </is>
-      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="19" t="n"/>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1" s="11">
       <c r="A7" s="14" t="n"/>
       <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="19" t="inlineStr">
-        <is>
-          <t>LG75UP77set</t>
-        </is>
-      </c>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="19" t="n"/>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1" s="11">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D8" s="19" t="inlineStr">
-        <is>
-          <t>فوم طقم رويال جاز المعدل</t>
-        </is>
-      </c>
+      <c r="C8" s="4" t="n"/>
+      <c r="D8" s="19" t="n"/>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -5175,17 +5014,17 @@
     </row>
     <row r="14" ht="18" customHeight="1" s="11">
       <c r="A14" s="36" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="37" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="19" t="inlineStr">
         <is>
-          <t>فكتوريا قاعدة ولوحة تحكم وحلة</t>
+          <t>زانوسى العبد 305</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -5195,11 +5034,11 @@
       <c r="A15" s="31" t="n"/>
       <c r="B15" s="34" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="19" t="inlineStr">
         <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
+          <t>صندوق سمك 25 ك</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -5208,56 +5047,32 @@
     <row r="16" ht="18" customHeight="1" s="11">
       <c r="A16" s="31" t="n"/>
       <c r="B16" s="34" t="n"/>
-      <c r="C16" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">دايو 11قدم المعدل </t>
-        </is>
-      </c>
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="19" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1" s="11">
       <c r="A17" s="31" t="n"/>
       <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D17" s="19" t="inlineStr">
-        <is>
-          <t>فوم طقم رويال جاز المعدل</t>
-        </is>
-      </c>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="19" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1" s="11">
       <c r="A18" s="31" t="n"/>
       <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D18" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="19" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1" s="11">
       <c r="A19" s="31" t="n"/>
       <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D19" s="19" t="inlineStr">
-        <is>
-          <t>فوم قاعده 60*60</t>
-        </is>
-      </c>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="19" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
@@ -5335,10 +5150,10 @@
     </row>
     <row r="25" ht="18" customHeight="1" s="11">
       <c r="A25" s="36" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B25" s="37" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="19" t="n"/>
@@ -5450,1247 +5265,17 @@
     </row>
     <row r="35" ht="18" customHeight="1" s="11">
       <c r="A35" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="B35" s="33" t="n"/>
-      <c r="C35" s="4" t="n"/>
-      <c r="D35" s="19" t="n"/>
-      <c r="E35" s="9" t="n"/>
-      <c r="F35" s="9" t="n"/>
-    </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n"/>
-      <c r="D36" s="19" t="n"/>
-      <c r="E36" s="9" t="n"/>
-      <c r="F36" s="9" t="n"/>
-    </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="19" t="n"/>
-      <c r="E37" s="9" t="n"/>
-      <c r="F37" s="9" t="n"/>
-    </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
-      <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
-      <c r="E38" s="9" t="n"/>
-      <c r="F38" s="9" t="n"/>
-    </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
-      <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
-      <c r="E39" s="9" t="n"/>
-      <c r="F39" s="9" t="n"/>
-    </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
-      <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
-      <c r="E40" s="9" t="n"/>
-      <c r="F40" s="9" t="n"/>
-    </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
-      <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
-      <c r="E41" s="9" t="n"/>
-      <c r="F41" s="9" t="n"/>
-    </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
-      <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
-      <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F42"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
-  <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D1" s="17" t="n">
-        <v>2022</v>
-      </c>
-      <c r="E1" s="3" t="n"/>
-      <c r="F1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
-        <is>
-          <t>اولا : نسبة التالف على الماكينات</t>
-        </is>
-      </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
-        <is>
-          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
-        </is>
-      </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
-        </is>
-      </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E3" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n">
-        <v>0.7781921996592531</v>
-      </c>
-      <c r="B4" s="40" t="n">
-        <v>0.6943525988625844</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>LG65UP81</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="n"/>
-      <c r="F4" s="9" t="n"/>
-    </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
-      <c r="C5" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D5" s="19" t="inlineStr">
-        <is>
-          <t>LG75UP77-front</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="n"/>
-      <c r="F5" s="9" t="n"/>
-    </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>اعلي نسبة توالف</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>OLED65cs6la</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="n"/>
-      <c r="F6" s="9" t="n"/>
-    </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="19" t="n"/>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-    </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="19" t="n"/>
-      <c r="E8" s="9" t="n"/>
-      <c r="F8" s="9" t="n"/>
-    </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B9" s="13" t="inlineStr">
-        <is>
-          <t>وسيط التوالف</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
-      <c r="E9" s="9" t="n"/>
-      <c r="F9" s="9" t="n"/>
-    </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
-      <c r="E10" s="9" t="n"/>
-      <c r="F10" s="9" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
-      <c r="E11" s="9" t="n"/>
-      <c r="F11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
-        </is>
-      </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
-        </is>
-      </c>
-      <c r="B13" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D13" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="37" t="n">
-        <v>7</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
-        </is>
-      </c>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-    </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
-      <c r="C15" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" s="33" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D15" s="19" t="inlineStr">
-        <is>
-          <t>oled55cs6la</t>
-        </is>
-      </c>
-      <c r="E15" s="9" t="n"/>
-      <c r="F15" s="9" t="n"/>
-    </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="C16" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
-        </is>
-      </c>
-      <c r="E16" s="9" t="n"/>
-      <c r="F16" s="9" t="n"/>
-    </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D17" s="19" t="inlineStr">
-        <is>
-          <t>OLED65cs6la</t>
-        </is>
-      </c>
-      <c r="E17" s="9" t="n"/>
-      <c r="F17" s="9" t="n"/>
-    </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D18" s="19" t="inlineStr">
-        <is>
-          <t>صندوق سمك 25 ك</t>
-        </is>
-      </c>
-      <c r="E18" s="9" t="n"/>
-      <c r="F18" s="9" t="n"/>
-    </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D19" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
-      <c r="E19" s="9" t="n"/>
-      <c r="F19" s="9" t="n"/>
-    </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
-      <c r="C20" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D20" s="19" t="inlineStr">
-        <is>
-          <t>فوم قاعده 60*60</t>
-        </is>
-      </c>
-      <c r="E20" s="9" t="n"/>
-      <c r="F20" s="9" t="n"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="19" t="n"/>
-      <c r="E21" s="9" t="n"/>
-      <c r="F21" s="9" t="n"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
-      <c r="E22" s="9" t="n"/>
-      <c r="F22" s="9" t="n"/>
-    </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
-        </is>
-      </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B24" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
-        </is>
-      </c>
-      <c r="C24" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D24" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E24" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F24" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n">
-        <v>13</v>
-      </c>
-      <c r="B25" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D25" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
-      <c r="E25" s="9" t="n"/>
-      <c r="F25" s="9" t="n"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="19" t="n"/>
-      <c r="E26" s="9" t="n"/>
-      <c r="F26" s="9" t="n"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="19" t="n"/>
-      <c r="E27" s="9" t="n"/>
-      <c r="F27" s="9" t="n"/>
-    </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
-      <c r="E28" s="9" t="n"/>
-      <c r="F28" s="9" t="n"/>
-    </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
-      <c r="E29" s="9" t="n"/>
-      <c r="F29" s="9" t="n"/>
-    </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
-      <c r="E30" s="9" t="n"/>
-      <c r="F30" s="9" t="n"/>
-    </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
-      <c r="E31" s="9" t="n"/>
-      <c r="F31" s="9" t="n"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
-      <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
-      <c r="E32" s="10" t="n"/>
-      <c r="F32" s="10" t="n"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
-        </is>
-      </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
-        </is>
-      </c>
-      <c r="C34" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D34" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E34" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F34" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n">
-        <v>13</v>
-      </c>
-      <c r="B35" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>4</v>
-      </c>
       <c r="D35" s="19" t="inlineStr">
         <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
-        </is>
-      </c>
-      <c r="E35" s="9" t="n"/>
-      <c r="F35" s="9" t="n"/>
-    </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D36" s="19" t="inlineStr">
-        <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
-        </is>
-      </c>
-      <c r="E36" s="9" t="n"/>
-      <c r="F36" s="9" t="n"/>
-    </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D37" s="19" t="inlineStr">
-        <is>
-          <t>OLED65cs6la</t>
-        </is>
-      </c>
-      <c r="E37" s="9" t="n"/>
-      <c r="F37" s="9" t="n"/>
-    </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
-      <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
-      <c r="E38" s="9" t="n"/>
-      <c r="F38" s="9" t="n"/>
-    </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
-      <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
-      <c r="E39" s="9" t="n"/>
-      <c r="F39" s="9" t="n"/>
-    </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
-      <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
-      <c r="E40" s="9" t="n"/>
-      <c r="F40" s="9" t="n"/>
-    </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
-      <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
-      <c r="E41" s="9" t="n"/>
-      <c r="F41" s="9" t="n"/>
-    </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
-      <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
-      <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F42"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
-  <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D1" s="17" t="n">
-        <v>2022</v>
-      </c>
-      <c r="E1" s="3" t="n"/>
-      <c r="F1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
-        <is>
-          <t>اولا : نسبة التالف على الماكينات</t>
-        </is>
-      </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
-        <is>
-          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
-        </is>
-      </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
-        </is>
-      </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E3" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n">
-        <v>0.7057502606464031</v>
-      </c>
-      <c r="B4" s="40" t="n">
-        <v>0.5666420300566642</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>LG65UP81</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="n"/>
-      <c r="F4" s="9" t="n"/>
-    </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
-      <c r="C5" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D5" s="19" t="inlineStr">
-        <is>
-          <t>70UQ80006LD</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="n"/>
-      <c r="F5" s="9" t="n"/>
-    </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>اعلي نسبة توالف</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>فوم قاعده 60*60</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="n"/>
-      <c r="F6" s="9" t="n"/>
-    </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="19" t="n"/>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-    </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="19" t="n"/>
-      <c r="E8" s="9" t="n"/>
-      <c r="F8" s="9" t="n"/>
-    </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B9" s="13" t="inlineStr">
-        <is>
-          <t>وسيط التوالف</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
-      <c r="E9" s="9" t="n"/>
-      <c r="F9" s="9" t="n"/>
-    </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
-      <c r="E10" s="9" t="n"/>
-      <c r="F10" s="9" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
-      <c r="E11" s="9" t="n"/>
-      <c r="F11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
-        </is>
-      </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
-        </is>
-      </c>
-      <c r="B13" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D13" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" s="37" t="n">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
-        </is>
-      </c>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-    </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
-      <c r="C15" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="19" t="inlineStr">
-        <is>
-          <t>oled55cs6la</t>
-        </is>
-      </c>
-      <c r="E15" s="9" t="n"/>
-      <c r="F15" s="9" t="n"/>
-    </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="C16" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
-      <c r="E16" s="9" t="n"/>
-      <c r="F16" s="9" t="n"/>
-    </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D17" s="19" t="inlineStr">
-        <is>
-          <t>فوم قاعده 60*60</t>
-        </is>
-      </c>
-      <c r="E17" s="9" t="n"/>
-      <c r="F17" s="9" t="n"/>
-    </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="19" t="n"/>
-      <c r="E18" s="9" t="n"/>
-      <c r="F18" s="9" t="n"/>
-    </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="19" t="n"/>
-      <c r="E19" s="9" t="n"/>
-      <c r="F19" s="9" t="n"/>
-    </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="19" t="n"/>
-      <c r="E20" s="9" t="n"/>
-      <c r="F20" s="9" t="n"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="19" t="n"/>
-      <c r="E21" s="9" t="n"/>
-      <c r="F21" s="9" t="n"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
-      <c r="E22" s="9" t="n"/>
-      <c r="F22" s="9" t="n"/>
-    </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
-        </is>
-      </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B24" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
-        </is>
-      </c>
-      <c r="C24" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D24" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E24" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F24" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n">
-        <v>12</v>
-      </c>
-      <c r="B25" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="19" t="n"/>
-      <c r="E25" s="9" t="n"/>
-      <c r="F25" s="9" t="n"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="19" t="n"/>
-      <c r="E26" s="9" t="n"/>
-      <c r="F26" s="9" t="n"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="19" t="n"/>
-      <c r="E27" s="9" t="n"/>
-      <c r="F27" s="9" t="n"/>
-    </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
-      <c r="E28" s="9" t="n"/>
-      <c r="F28" s="9" t="n"/>
-    </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
-      <c r="E29" s="9" t="n"/>
-      <c r="F29" s="9" t="n"/>
-    </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
-      <c r="E30" s="9" t="n"/>
-      <c r="F30" s="9" t="n"/>
-    </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
-      <c r="E31" s="9" t="n"/>
-      <c r="F31" s="9" t="n"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
-      <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
-      <c r="E32" s="10" t="n"/>
-      <c r="F32" s="10" t="n"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
-        </is>
-      </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
-        </is>
-      </c>
-      <c r="C34" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D34" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E34" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F34" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n">
-        <v>12</v>
-      </c>
-      <c r="B35" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D35" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
+          <t>زانوسى العبد 305</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -6704,7 +5289,7 @@
       </c>
       <c r="D36" s="19" t="inlineStr">
         <is>
-          <t>LG65UP81</t>
+          <t>LG65UM73</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
@@ -6713,677 +5298,28 @@
     <row r="37" ht="18" customHeight="1" s="11">
       <c r="A37" s="31" t="n"/>
       <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="19" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D37" s="19" t="inlineStr">
+        <is>
+          <t>LG43LM63-UM73</t>
+        </is>
+      </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1" s="11">
       <c r="A38" s="31" t="n"/>
       <c r="B38" s="34" t="n"/>
-      <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
-      <c r="E38" s="9" t="n"/>
-      <c r="F38" s="9" t="n"/>
-    </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
-      <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
-      <c r="E39" s="9" t="n"/>
-      <c r="F39" s="9" t="n"/>
-    </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
-      <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
-      <c r="E40" s="9" t="n"/>
-      <c r="F40" s="9" t="n"/>
-    </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
-      <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
-      <c r="E41" s="9" t="n"/>
-      <c r="F41" s="9" t="n"/>
-    </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
-      <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
-      <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
-  <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D1" s="17" t="n">
-        <v>2022</v>
-      </c>
-      <c r="E1" s="3" t="n"/>
-      <c r="F1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
-        <is>
-          <t>اولا : نسبة التالف على الماكينات</t>
-        </is>
-      </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
-        <is>
-          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
-        </is>
-      </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
-        </is>
-      </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E3" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n">
-        <v>1.007026641115244</v>
-      </c>
-      <c r="B4" s="40" t="n">
-        <v>0.919954002299885</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>فوم صندوق سمك 35 ك</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="n"/>
-      <c r="F4" s="9" t="n"/>
-    </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
-      <c r="C5" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="n"/>
-      <c r="F5" s="9" t="n"/>
-    </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>اعلي نسبة توالف</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>LG65UP81</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="n"/>
-      <c r="F6" s="9" t="n"/>
-    </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D7" s="19" t="inlineStr">
-        <is>
-          <t>LG65UP77_TB</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-    </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D8" s="19" t="inlineStr">
-        <is>
-          <t>زانوسي 70 سم -2 (قاعدة ، كفر)</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="n"/>
-      <c r="F8" s="9" t="n"/>
-    </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B9" s="13" t="inlineStr">
-        <is>
-          <t>وسيط التوالف</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
-      <c r="E9" s="9" t="n"/>
-      <c r="F9" s="9" t="n"/>
-    </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
-      <c r="E10" s="9" t="n"/>
-      <c r="F10" s="9" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
-      <c r="E11" s="9" t="n"/>
-      <c r="F11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
-        </is>
-      </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
-        </is>
-      </c>
-      <c r="B13" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D13" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n">
-        <v>8</v>
-      </c>
-      <c r="B14" s="37" t="n">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
-        </is>
-      </c>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-    </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
-      <c r="C15" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="19" t="inlineStr">
-        <is>
-          <t>oled55cs6la</t>
-        </is>
-      </c>
-      <c r="E15" s="9" t="n"/>
-      <c r="F15" s="9" t="n"/>
-    </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="C16" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t>فوم صندوق سمك 35 ك</t>
-        </is>
-      </c>
-      <c r="E16" s="9" t="n"/>
-      <c r="F16" s="9" t="n"/>
-    </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D17" s="19" t="inlineStr">
-        <is>
-          <t>LG65UP77_TB</t>
-        </is>
-      </c>
-      <c r="E17" s="9" t="n"/>
-      <c r="F17" s="9" t="n"/>
-    </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>46</v>
-      </c>
-      <c r="D18" s="19" t="inlineStr">
-        <is>
-          <t>جانب حماية يمين / شمال</t>
-        </is>
-      </c>
-      <c r="E18" s="9" t="n"/>
-      <c r="F18" s="9" t="n"/>
-    </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D19" s="19" t="inlineStr">
-        <is>
-          <t>زانوسي 70 سم -2 (قاعدة ، كفر)</t>
-        </is>
-      </c>
-      <c r="E19" s="9" t="n"/>
-      <c r="F19" s="9" t="n"/>
-    </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
-      <c r="C20" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D20" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
-      <c r="E20" s="9" t="n"/>
-      <c r="F20" s="9" t="n"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
-      <c r="C21" s="4" t="n">
+      <c r="C38" s="4" t="n">
         <v>49</v>
       </c>
-      <c r="D21" s="19" t="inlineStr">
-        <is>
-          <t>فوم قاعده 60*60</t>
-        </is>
-      </c>
-      <c r="E21" s="9" t="n"/>
-      <c r="F21" s="9" t="n"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
-      <c r="E22" s="9" t="n"/>
-      <c r="F22" s="9" t="n"/>
-    </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
-        </is>
-      </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B24" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
-        </is>
-      </c>
-      <c r="C24" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D24" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E24" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F24" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n">
-        <v>11</v>
-      </c>
-      <c r="B25" s="37" t="n">
-        <v/>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="D25" s="19" t="inlineStr">
-        <is>
-          <t>سخان غاز 6لتر</t>
-        </is>
-      </c>
-      <c r="E25" s="9" t="n"/>
-      <c r="F25" s="9" t="n"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
-      <c r="C26" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D26" s="19" t="inlineStr">
-        <is>
-          <t>زانوسي 70 سم -2 (قاعدة ، كفر)</t>
-        </is>
-      </c>
-      <c r="E26" s="9" t="n"/>
-      <c r="F26" s="9" t="n"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
-      <c r="C27" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D27" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
-      <c r="E27" s="9" t="n"/>
-      <c r="F27" s="9" t="n"/>
-    </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
-      <c r="E28" s="9" t="n"/>
-      <c r="F28" s="9" t="n"/>
-    </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
-      <c r="E29" s="9" t="n"/>
-      <c r="F29" s="9" t="n"/>
-    </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
-      <c r="E30" s="9" t="n"/>
-      <c r="F30" s="9" t="n"/>
-    </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
-      <c r="E31" s="9" t="n"/>
-      <c r="F31" s="9" t="n"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
-      <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
-      <c r="E32" s="10" t="n"/>
-      <c r="F32" s="10" t="n"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
-        </is>
-      </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
-        </is>
-      </c>
-      <c r="C34" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D34" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E34" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F34" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n">
-        <v>11</v>
-      </c>
-      <c r="B35" s="33" t="n">
-        <v>5</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D35" s="19" t="inlineStr">
-        <is>
-          <t>oled55cs6la</t>
-        </is>
-      </c>
-      <c r="E35" s="9" t="n"/>
-      <c r="F35" s="9" t="n"/>
-    </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D36" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
-        </is>
-      </c>
-      <c r="E36" s="9" t="n"/>
-      <c r="F36" s="9" t="n"/>
-    </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="19" t="n"/>
-      <c r="E37" s="9" t="n"/>
-      <c r="F37" s="9" t="n"/>
-    </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
-      <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
+      <c r="D38" s="19" t="inlineStr">
+        <is>
+          <t>طقم سخان بلونايل ذو 4 اطقم</t>
+        </is>
+      </c>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>

</xml_diff>

<commit_message>
befor remove functions not used
</commit_message>
<xml_diff>
--- a/apps/analysis/formats/QC_molds_daily_summary.xlsx
+++ b/apps/analysis/formats/QC_molds_daily_summary.xlsx
@@ -3,22 +3,20 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="1" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="daily" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="6" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="11" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="daily" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="3" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="AccessDatabase" hidden="1">"C:\Documents and Settings\Administrator\My Documents\BITUNIL\FINANCE\SAMEER\Cost StudyHB.mdb"</definedName>
@@ -45,7 +43,7 @@
     <definedName name="الاوزان">'[5]0'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'daily'!$A$2:$F$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -475,7 +473,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" readingOrder="2"/>
@@ -503,7 +501,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
@@ -671,7 +668,7 @@
             <v>UCI</v>
           </cell>
           <cell r="C4" t="str">
-            <v xml:space="preserve">  chili paste </v>
+            <v>chili paste</v>
           </cell>
           <cell r="E4" t="str">
             <v>Al Gawhara</v>
@@ -732,7 +729,7 @@
         </row>
         <row r="6">
           <cell r="C6" t="str">
-            <v xml:space="preserve">canned tomato paste </v>
+            <v>canned tomato paste</v>
           </cell>
           <cell r="E6" t="str">
             <v>Bahiya</v>
@@ -796,7 +793,7 @@
             <v>7.5%:10%</v>
           </cell>
           <cell r="I8" t="str">
-            <v xml:space="preserve">plastic barrel </v>
+            <v>plastic barrel</v>
           </cell>
           <cell r="K8">
             <v>4</v>
@@ -859,7 +856,7 @@
         </row>
         <row r="11">
           <cell r="C11" t="str">
-            <v xml:space="preserve">Peach pulp </v>
+            <v>Peach pulp</v>
           </cell>
           <cell r="E11" t="str">
             <v>Byza</v>
@@ -885,7 +882,7 @@
             <v>Promotion</v>
           </cell>
           <cell r="E12" t="str">
-            <v xml:space="preserve">C.B </v>
+            <v>C.B</v>
           </cell>
           <cell r="G12" t="str">
             <v>Heart</v>
@@ -902,7 +899,7 @@
             <v>Raspberry Bulb</v>
           </cell>
           <cell r="E13" t="str">
-            <v xml:space="preserve">chili paste </v>
+            <v>chili paste</v>
           </cell>
           <cell r="G13" t="str">
             <v>Penne</v>
@@ -933,7 +930,7 @@
         </row>
         <row r="15">
           <cell r="C15" t="str">
-            <v xml:space="preserve">Tomato Paste </v>
+            <v>Tomato Paste</v>
           </cell>
           <cell r="E15" t="str">
             <v>Guava Bulb</v>
@@ -1049,7 +1046,7 @@
         </row>
         <row r="25">
           <cell r="E25" t="str">
-            <v xml:space="preserve">lachaine 140 gm </v>
+            <v>lachaine 140 gm</v>
           </cell>
           <cell r="G25" t="str">
             <v>Vermicelli</v>
@@ -1060,7 +1057,7 @@
         </row>
         <row r="26">
           <cell r="E26" t="str">
-            <v xml:space="preserve">lachaine 70 gm </v>
+            <v>lachaine 70 gm</v>
           </cell>
           <cell r="G26" t="str">
             <v>Wheel</v>
@@ -1071,7 +1068,7 @@
         </row>
         <row r="27">
           <cell r="E27" t="str">
-            <v xml:space="preserve">lachaine 800 gm </v>
+            <v>lachaine 800 gm</v>
           </cell>
           <cell r="K27">
             <v>225</v>
@@ -1079,7 +1076,7 @@
         </row>
         <row r="28">
           <cell r="E28" t="str">
-            <v xml:space="preserve">Lakwam 140 gm </v>
+            <v>Lakwam 140 gm</v>
           </cell>
           <cell r="K28">
             <v>250</v>
@@ -1087,7 +1084,7 @@
         </row>
         <row r="29">
           <cell r="E29" t="str">
-            <v xml:space="preserve">Lakwam 70 gm </v>
+            <v>Lakwam 70 gm</v>
           </cell>
           <cell r="K29">
             <v>1000</v>
@@ -1095,22 +1092,22 @@
         </row>
         <row r="30">
           <cell r="E30" t="str">
-            <v xml:space="preserve">Lakwam 800 gm </v>
+            <v>Lakwam 800 gm</v>
           </cell>
         </row>
         <row r="31">
           <cell r="E31" t="str">
-            <v xml:space="preserve">Laprier 140 gm </v>
+            <v>Laprier 140 gm</v>
           </cell>
         </row>
         <row r="32">
           <cell r="E32" t="str">
-            <v xml:space="preserve">Laprier 70gm </v>
+            <v>Laprier 70gm</v>
           </cell>
         </row>
         <row r="33">
           <cell r="E33" t="str">
-            <v xml:space="preserve">Laprier 800 gm </v>
+            <v>Laprier 800 gm</v>
           </cell>
         </row>
         <row r="34">
@@ -1140,17 +1137,17 @@
         </row>
         <row r="39">
           <cell r="E39" t="str">
-            <v xml:space="preserve">Rosso 140 gm </v>
+            <v>Rosso 140 gm</v>
           </cell>
         </row>
         <row r="40">
           <cell r="E40" t="str">
-            <v xml:space="preserve">Rosso 380 gm </v>
+            <v>Rosso 380 gm</v>
           </cell>
         </row>
         <row r="41">
           <cell r="E41" t="str">
-            <v xml:space="preserve">Rosso 70 gm </v>
+            <v>Rosso 70 gm</v>
           </cell>
         </row>
         <row r="42">
@@ -1279,7 +1276,7 @@
       <sheetData sheetId="11">
         <row r="26">
           <cell r="C26" t="str">
-            <v xml:space="preserve">Fixed </v>
+            <v>Fixed</v>
           </cell>
         </row>
         <row r="27">
@@ -1823,15 +1820,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
+    <col width="26.625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.625" customWidth="1" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="21" min="4" max="4"/>
+    <col width="28.875" customWidth="1" min="5" max="5"/>
+    <col width="31.875" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
+    <row r="1" ht="18.75" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
@@ -1839,33 +1836,33 @@
       </c>
       <c r="B1" s="2" t="n"/>
       <c r="C1" s="2" t="n"/>
-      <c r="D1" s="17" t="n"/>
+      <c r="D1" s="16" t="n"/>
       <c r="E1" s="3" t="n"/>
       <c r="F1" s="3" t="n"/>
     </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
+    <row r="2" ht="21" customHeight="1" thickBot="1">
+      <c r="A2" s="37" t="inlineStr">
         <is>
           <t>اولا : نسبة التالف على الماكينات</t>
         </is>
       </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
+      <c r="B2" s="28" t="n"/>
+      <c r="C2" s="23" t="inlineStr">
         <is>
           <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
         </is>
       </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="D2" s="24" t="n"/>
+      <c r="E2" s="24" t="n"/>
+      <c r="F2" s="24" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
         </is>
@@ -1875,7 +1872,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D3" s="18" t="inlineStr">
+      <c r="D3" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -1891,109 +1888,109 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n"/>
-      <c r="B4" s="40" t="n"/>
+    <row r="4" ht="21.75" customHeight="1">
+      <c r="A4" s="38" t="n"/>
+      <c r="B4" s="39" t="n"/>
       <c r="C4" s="4" t="n"/>
-      <c r="D4" s="19" t="n"/>
+      <c r="D4" s="18" t="n"/>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
     </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
+    <row r="5" ht="21.75" customHeight="1">
+      <c r="A5" s="30" t="n"/>
+      <c r="B5" s="33" t="n"/>
       <c r="C5" s="4" t="n"/>
-      <c r="D5" s="19" t="n"/>
+      <c r="D5" s="18" t="n"/>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
+    <row r="6" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>لماكينة</t>
         </is>
       </c>
-      <c r="B6" s="13" t="inlineStr">
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
       <c r="C6" s="4" t="n"/>
-      <c r="D6" s="19" t="n"/>
+      <c r="D6" s="18" t="n"/>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
+    <row r="7" ht="21.75" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="15" t="n"/>
       <c r="C7" s="4" t="n"/>
-      <c r="D7" s="19" t="n"/>
+      <c r="D7" s="18" t="n"/>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
+    <row r="8" ht="21.75" customHeight="1">
+      <c r="A8" s="13" t="n"/>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="4" t="n"/>
-      <c r="D8" s="19" t="n"/>
+      <c r="D8" s="18" t="n"/>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
+    <row r="9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A9" s="11" t="inlineStr">
         <is>
           <t>لماكينة</t>
         </is>
       </c>
-      <c r="B9" s="13" t="inlineStr">
+      <c r="B9" s="12" t="inlineStr">
         <is>
           <t>وسيط التوالف</t>
         </is>
       </c>
       <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
+      <c r="D9" s="18" t="n"/>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="15" t="n"/>
       <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
+      <c r="D10" s="18" t="n"/>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
+    <row r="11" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="15" t="n"/>
       <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
+      <c r="D11" s="19" t="n"/>
       <c r="E11" s="9" t="n"/>
       <c r="F11" s="9" t="n"/>
     </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
+    <row r="12" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A12" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
         </is>
       </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
+      <c r="B12" s="28" t="n"/>
+      <c r="C12" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
+      <c r="D12" s="26" t="n"/>
+      <c r="E12" s="26" t="n"/>
+      <c r="F12" s="26" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="A13" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
         </is>
       </c>
-      <c r="B13" s="13" t="inlineStr">
+      <c r="B13" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
         </is>
@@ -2003,7 +2000,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D13" s="18" t="inlineStr">
+      <c r="D13" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -2019,101 +2016,101 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n"/>
-      <c r="B14" s="37" t="n"/>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="35" t="n"/>
+      <c r="B14" s="36" t="n"/>
       <c r="C14" s="4" t="n"/>
-      <c r="D14" s="19" t="n"/>
+      <c r="D14" s="18" t="n"/>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
+    <row r="15" ht="18" customHeight="1">
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="33" t="n"/>
       <c r="C15" s="4" t="n"/>
-      <c r="D15" s="19" t="n"/>
+      <c r="D15" s="18" t="n"/>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="33" t="n"/>
       <c r="C16" s="4" t="n"/>
-      <c r="D16" s="19" t="n"/>
+      <c r="D16" s="18" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
+    <row r="17" ht="18" customHeight="1">
+      <c r="A17" s="30" t="n"/>
+      <c r="B17" s="33" t="n"/>
       <c r="C17" s="4" t="n"/>
-      <c r="D17" s="19" t="n"/>
+      <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="30" t="n"/>
+      <c r="B18" s="33" t="n"/>
       <c r="C18" s="4" t="n"/>
-      <c r="D18" s="19" t="n"/>
+      <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="30" t="n"/>
+      <c r="B19" s="33" t="n"/>
       <c r="C19" s="4" t="n"/>
-      <c r="D19" s="19" t="n"/>
+      <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="30" t="n"/>
+      <c r="B20" s="33" t="n"/>
       <c r="C20" s="4" t="n"/>
-      <c r="D20" s="19" t="n"/>
+      <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="30" t="n"/>
+      <c r="B21" s="33" t="n"/>
       <c r="C21" s="4" t="n"/>
-      <c r="D21" s="19" t="n"/>
+      <c r="D21" s="18" t="n"/>
       <c r="E21" s="9" t="n"/>
       <c r="F21" s="9" t="n"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
+    <row r="22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A22" s="22" t="n"/>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
+      <c r="D22" s="20" t="n"/>
       <c r="E22" s="9" t="n"/>
       <c r="F22" s="9" t="n"/>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
+    <row r="23" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A23" s="27" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
         </is>
       </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
+      <c r="B23" s="28" t="n"/>
+      <c r="C23" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="D23" s="26" t="n"/>
+      <c r="E23" s="26" t="n"/>
+      <c r="F23" s="26" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
         </is>
       </c>
-      <c r="B24" s="13" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
         </is>
@@ -2123,7 +2120,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D24" s="18" t="inlineStr">
+      <c r="D24" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -2139,92 +2136,92 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n"/>
-      <c r="B25" s="37" t="n"/>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="35" t="n"/>
+      <c r="B25" s="36" t="n"/>
       <c r="C25" s="4" t="n"/>
-      <c r="D25" s="19" t="n"/>
+      <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="30" t="n"/>
+      <c r="B26" s="33" t="n"/>
       <c r="C26" s="4" t="n"/>
-      <c r="D26" s="19" t="n"/>
+      <c r="D26" s="18" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
+    <row r="27" ht="18" customHeight="1">
+      <c r="A27" s="30" t="n"/>
+      <c r="B27" s="33" t="n"/>
       <c r="C27" s="4" t="n"/>
-      <c r="D27" s="19" t="n"/>
+      <c r="D27" s="18" t="n"/>
       <c r="E27" s="9" t="n"/>
       <c r="F27" s="9" t="n"/>
     </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
+    <row r="28" ht="18" customHeight="1">
+      <c r="A28" s="30" t="n"/>
+      <c r="B28" s="33" t="n"/>
       <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
+      <c r="D28" s="18" t="n"/>
       <c r="E28" s="9" t="n"/>
       <c r="F28" s="9" t="n"/>
     </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
+    <row r="29" ht="18" customHeight="1">
+      <c r="A29" s="30" t="n"/>
+      <c r="B29" s="33" t="n"/>
       <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
+      <c r="D29" s="18" t="n"/>
       <c r="E29" s="9" t="n"/>
       <c r="F29" s="9" t="n"/>
     </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="30" t="n"/>
+      <c r="B30" s="33" t="n"/>
       <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
+      <c r="D30" s="18" t="n"/>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="9" t="n"/>
     </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="30" t="n"/>
+      <c r="B31" s="33" t="n"/>
       <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
+      <c r="D31" s="18" t="n"/>
       <c r="E31" s="9" t="n"/>
       <c r="F31" s="9" t="n"/>
     </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
+    <row r="32" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A32" s="30" t="n"/>
+      <c r="B32" s="33" t="n"/>
       <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
+      <c r="D32" s="19" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
     </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
+    <row r="33" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A33" s="27" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
         </is>
       </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
+      <c r="B33" s="28" t="n"/>
+      <c r="C33" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
+      <c r="D33" s="26" t="n"/>
+      <c r="E33" s="26" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1">
+      <c r="A34" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
         </is>
       </c>
-      <c r="B34" s="12" t="inlineStr">
+      <c r="B34" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
         </is>
@@ -2234,7 +2231,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D34" s="18" t="inlineStr">
+      <c r="D34" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -2250,67 +2247,67 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n"/>
-      <c r="B35" s="33" t="n"/>
+    <row r="35" ht="18" customHeight="1">
+      <c r="A35" s="29" t="n"/>
+      <c r="B35" s="32" t="n"/>
       <c r="C35" s="4" t="n"/>
-      <c r="D35" s="19" t="n"/>
+      <c r="D35" s="18" t="n"/>
       <c r="E35" s="9" t="n"/>
       <c r="F35" s="9" t="n"/>
     </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
+    <row r="36" ht="18" customHeight="1">
+      <c r="A36" s="30" t="n"/>
+      <c r="B36" s="33" t="n"/>
       <c r="C36" s="4" t="n"/>
-      <c r="D36" s="19" t="n"/>
+      <c r="D36" s="18" t="n"/>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
+    <row r="37" ht="18" customHeight="1">
+      <c r="A37" s="30" t="n"/>
+      <c r="B37" s="33" t="n"/>
       <c r="C37" s="4" t="n"/>
-      <c r="D37" s="19" t="n"/>
+      <c r="D37" s="18" t="n"/>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
+    <row r="38" ht="18" customHeight="1">
+      <c r="A38" s="30" t="n"/>
+      <c r="B38" s="33" t="n"/>
       <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
+      <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
+    <row r="39" ht="18" customHeight="1">
+      <c r="A39" s="30" t="n"/>
+      <c r="B39" s="33" t="n"/>
       <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
+      <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
+    <row r="40" ht="18" customHeight="1">
+      <c r="A40" s="30" t="n"/>
+      <c r="B40" s="33" t="n"/>
       <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
+      <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
+    <row r="41" ht="18" customHeight="1">
+      <c r="A41" s="30" t="n"/>
+      <c r="B41" s="33" t="n"/>
       <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
+      <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
+    <row r="42" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A42" s="31" t="n"/>
+      <c r="B42" s="34" t="n"/>
       <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
+      <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
     </row>
@@ -2352,21 +2349,21 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F42" sqref="A1:F42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
+    <col width="26.625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.625" customWidth="1" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="21" min="4" max="4"/>
+    <col width="28.875" customWidth="1" min="5" max="5"/>
+    <col width="31.875" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
+    <row r="1" ht="18.75" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
@@ -2374,41 +2371,41 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D1" s="17" t="n">
-        <v>2022</v>
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="n">
+        <v>2023</v>
       </c>
       <c r="E1" s="3" t="n"/>
       <c r="F1" s="3" t="n"/>
     </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
+    <row r="2" ht="21" customHeight="1" thickBot="1">
+      <c r="A2" s="37" t="inlineStr">
         <is>
           <t>اولا : نسبة التالف على الماكينات</t>
         </is>
       </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
+      <c r="B2" s="28" t="n"/>
+      <c r="C2" s="23" t="inlineStr">
         <is>
           <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
         </is>
       </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="D2" s="24" t="n"/>
+      <c r="E2" s="24" t="n"/>
+      <c r="F2" s="24" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
         </is>
@@ -2418,7 +2415,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D3" s="18" t="inlineStr">
+      <c r="D3" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -2434,143 +2431,125 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n">
-        <v>0.7635200386286818</v>
-      </c>
-      <c r="B4" s="40" t="n">
-        <v>0.7398501803384815</v>
+    <row r="4" ht="21.75" customHeight="1">
+      <c r="A4" s="38" t="n">
+        <v>0.5245319561007101</v>
+      </c>
+      <c r="B4" s="39" t="n">
+        <v>0.4118416589951063</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+        <v>6</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>LG 65UP77 FRONT</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
     </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
+    <row r="5" ht="21.75" customHeight="1">
+      <c r="A5" s="30" t="n"/>
+      <c r="B5" s="33" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
+        <v>30</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>زانوسي العبد 309 - 314</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
+    <row r="6" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>لماكينة</t>
         </is>
       </c>
-      <c r="B6" s="13" t="inlineStr">
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>LG75UP77-front</t>
-        </is>
-      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="18" t="n"/>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D7" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
+    <row r="7" ht="21.75" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="15" t="n"/>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="18" t="n"/>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n">
-        <v>46</v>
-      </c>
-      <c r="D8" s="19" t="inlineStr">
-        <is>
-          <t>جانب حماية يمين / شمال</t>
-        </is>
-      </c>
+    <row r="8" ht="21.75" customHeight="1">
+      <c r="A8" s="13" t="n"/>
+      <c r="B8" s="14" t="n"/>
+      <c r="C8" s="4" t="n"/>
+      <c r="D8" s="18" t="n"/>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
+    <row r="9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A9" s="11" t="inlineStr">
         <is>
           <t>لماكينة</t>
         </is>
       </c>
-      <c r="B9" s="13" t="inlineStr">
+      <c r="B9" s="12" t="inlineStr">
         <is>
           <t>وسيط التوالف</t>
         </is>
       </c>
       <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
+      <c r="D9" s="18" t="n"/>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="15" t="n"/>
       <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
+      <c r="D10" s="18" t="n"/>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
+    <row r="11" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="15" t="n"/>
       <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
+      <c r="D11" s="19" t="n"/>
       <c r="E11" s="9" t="n"/>
       <c r="F11" s="9" t="n"/>
     </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
+    <row r="12" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A12" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
         </is>
       </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
+      <c r="B12" s="28" t="n"/>
+      <c r="C12" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
+      <c r="D12" s="26" t="n"/>
+      <c r="E12" s="26" t="n"/>
+      <c r="F12" s="26" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="A13" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
         </is>
       </c>
-      <c r="B13" s="13" t="inlineStr">
+      <c r="B13" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
         </is>
@@ -2580,7 +2559,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D13" s="18" t="inlineStr">
+      <c r="D13" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -2596,135 +2575,117 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n">
-        <v>11</v>
-      </c>
-      <c r="B14" s="37" t="n">
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="35" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>oled55cs6la</t>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 25 ك</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
+    <row r="15" ht="18" customHeight="1">
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="33" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D15" s="19" t="inlineStr">
-        <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
+        <v>6</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>LG 65UP77 FRONT</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="C16" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="33" t="n"/>
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="18" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D17" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+    <row r="17" ht="18" customHeight="1">
+      <c r="A17" s="30" t="n"/>
+      <c r="B17" s="33" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D18" s="19" t="inlineStr">
-        <is>
-          <t>فوم قاعده 60*60</t>
-        </is>
-      </c>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="30" t="n"/>
+      <c r="B18" s="33" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="30" t="n"/>
+      <c r="B19" s="33" t="n"/>
       <c r="C19" s="4" t="n"/>
-      <c r="D19" s="19" t="n"/>
+      <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="30" t="n"/>
+      <c r="B20" s="33" t="n"/>
       <c r="C20" s="4" t="n"/>
-      <c r="D20" s="19" t="n"/>
+      <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="30" t="n"/>
+      <c r="B21" s="33" t="n"/>
       <c r="C21" s="4" t="n"/>
-      <c r="D21" s="19" t="n"/>
+      <c r="D21" s="18" t="n"/>
       <c r="E21" s="9" t="n"/>
       <c r="F21" s="9" t="n"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
+    <row r="22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A22" s="22" t="n"/>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
+      <c r="D22" s="20" t="n"/>
       <c r="E22" s="9" t="n"/>
       <c r="F22" s="9" t="n"/>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
+    <row r="23" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A23" s="27" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
         </is>
       </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
+      <c r="B23" s="28" t="n"/>
+      <c r="C23" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="D23" s="26" t="n"/>
+      <c r="E23" s="26" t="n"/>
+      <c r="F23" s="26" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
         </is>
       </c>
-      <c r="B24" s="13" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
         </is>
@@ -2734,7 +2695,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D24" s="18" t="inlineStr">
+      <c r="D24" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -2750,96 +2711,94 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n">
-        <v>13</v>
-      </c>
-      <c r="B25" s="37" t="n">
-        <v>0</v>
-      </c>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="35" t="n">
+        <v>6</v>
+      </c>
+      <c r="B25" s="36" t="n"/>
       <c r="C25" s="4" t="n"/>
-      <c r="D25" s="19" t="n"/>
+      <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="30" t="n"/>
+      <c r="B26" s="33" t="n"/>
       <c r="C26" s="4" t="n"/>
-      <c r="D26" s="19" t="n"/>
+      <c r="D26" s="18" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
+    <row r="27" ht="18" customHeight="1">
+      <c r="A27" s="30" t="n"/>
+      <c r="B27" s="33" t="n"/>
       <c r="C27" s="4" t="n"/>
-      <c r="D27" s="19" t="n"/>
+      <c r="D27" s="18" t="n"/>
       <c r="E27" s="9" t="n"/>
       <c r="F27" s="9" t="n"/>
     </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
+    <row r="28" ht="18" customHeight="1">
+      <c r="A28" s="30" t="n"/>
+      <c r="B28" s="33" t="n"/>
       <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
+      <c r="D28" s="18" t="n"/>
       <c r="E28" s="9" t="n"/>
       <c r="F28" s="9" t="n"/>
     </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
+    <row r="29" ht="18" customHeight="1">
+      <c r="A29" s="30" t="n"/>
+      <c r="B29" s="33" t="n"/>
       <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
+      <c r="D29" s="18" t="n"/>
       <c r="E29" s="9" t="n"/>
       <c r="F29" s="9" t="n"/>
     </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="30" t="n"/>
+      <c r="B30" s="33" t="n"/>
       <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
+      <c r="D30" s="18" t="n"/>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="9" t="n"/>
     </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="30" t="n"/>
+      <c r="B31" s="33" t="n"/>
       <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
+      <c r="D31" s="18" t="n"/>
       <c r="E31" s="9" t="n"/>
       <c r="F31" s="9" t="n"/>
     </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
+    <row r="32" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A32" s="30" t="n"/>
+      <c r="B32" s="33" t="n"/>
       <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
+      <c r="D32" s="19" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
     </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
+    <row r="33" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A33" s="27" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
         </is>
       </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
+      <c r="B33" s="28" t="n"/>
+      <c r="C33" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
+      <c r="D33" s="26" t="n"/>
+      <c r="E33" s="26" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1">
+      <c r="A34" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
         </is>
       </c>
-      <c r="B34" s="12" t="inlineStr">
+      <c r="B34" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
         </is>
@@ -2849,7 +2808,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D34" s="18" t="inlineStr">
+      <c r="D34" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -2865,89 +2824,89 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n">
-        <v>13</v>
-      </c>
-      <c r="B35" s="33" t="n">
+    <row r="35" ht="18" customHeight="1">
+      <c r="A35" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="B35" s="32" t="n">
         <v>3</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="19" t="inlineStr">
-        <is>
-          <t>LG43LM63-UM73</t>
+        <v>3</v>
+      </c>
+      <c r="D35" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة غسالة Lg</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
       <c r="F35" s="9" t="n"/>
     </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
+    <row r="36" ht="18" customHeight="1">
+      <c r="A36" s="30" t="n"/>
+      <c r="B36" s="33" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D36" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
+        <v>9</v>
+      </c>
+      <c r="D36" s="18" t="inlineStr">
+        <is>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
+    <row r="37" ht="18" customHeight="1">
+      <c r="A37" s="30" t="n"/>
+      <c r="B37" s="33" t="n"/>
       <c r="C37" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D37" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
+        <v>26</v>
+      </c>
+      <c r="D37" s="18" t="inlineStr">
+        <is>
+          <t>فوم كوش 152</t>
         </is>
       </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
+    <row r="38" ht="18" customHeight="1">
+      <c r="A38" s="30" t="n"/>
+      <c r="B38" s="33" t="n"/>
       <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
+      <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
+    <row r="39" ht="18" customHeight="1">
+      <c r="A39" s="30" t="n"/>
+      <c r="B39" s="33" t="n"/>
       <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
+      <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
+    <row r="40" ht="18" customHeight="1">
+      <c r="A40" s="30" t="n"/>
+      <c r="B40" s="33" t="n"/>
       <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
+      <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
+    <row r="41" ht="18" customHeight="1">
+      <c r="A41" s="30" t="n"/>
+      <c r="B41" s="33" t="n"/>
       <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
+      <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
+    <row r="42" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A42" s="31" t="n"/>
+      <c r="B42" s="34" t="n"/>
       <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
+      <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
     </row>
@@ -2983,21 +2942,21 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
+    <col width="26.625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.625" customWidth="1" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="21" min="4" max="4"/>
+    <col width="28.875" customWidth="1" min="5" max="5"/>
+    <col width="31.875" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
+    <row r="1" ht="18.75" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
@@ -3005,41 +2964,41 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D1" s="17" t="n">
-        <v>2022</v>
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="n">
+        <v>2023</v>
       </c>
       <c r="E1" s="3" t="n"/>
       <c r="F1" s="3" t="n"/>
     </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
+    <row r="2" ht="21" customHeight="1" thickBot="1">
+      <c r="A2" s="37" t="inlineStr">
         <is>
           <t>اولا : نسبة التالف على الماكينات</t>
         </is>
       </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
+      <c r="B2" s="28" t="n"/>
+      <c r="C2" s="23" t="inlineStr">
         <is>
           <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
         </is>
       </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="D2" s="24" t="n"/>
+      <c r="E2" s="24" t="n"/>
+      <c r="F2" s="24" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
         </is>
@@ -3049,7 +3008,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D3" s="18" t="inlineStr">
+      <c r="D3" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -3065,119 +3024,131 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n">
-        <v>0.7839313572542903</v>
-      </c>
-      <c r="B4" s="40" t="n">
-        <v>0.7853403141361256</v>
+    <row r="4" ht="21.75" customHeight="1">
+      <c r="A4" s="38" t="n">
+        <v>0.712523979172376</v>
+      </c>
+      <c r="B4" s="39" t="n">
+        <v>0.828438017773761</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>70UQ80006LD</t>
+        <v>3</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>صندوق 10 ك فلات</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
     </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="19" t="n"/>
+    <row r="5" ht="21.75" customHeight="1">
+      <c r="A5" s="30" t="n"/>
+      <c r="B5" s="33" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>زانوسى العبد 305-جديدة</t>
+        </is>
+      </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
+    <row r="6" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>لماكينة</t>
         </is>
       </c>
-      <c r="B6" s="13" t="inlineStr">
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="19" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
+    <row r="7" ht="21.75" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="15" t="n"/>
       <c r="C7" s="4" t="n"/>
-      <c r="D7" s="19" t="n"/>
+      <c r="D7" s="18" t="n"/>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
+    <row r="8" ht="21.75" customHeight="1">
+      <c r="A8" s="13" t="n"/>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="4" t="n"/>
-      <c r="D8" s="19" t="n"/>
+      <c r="D8" s="18" t="n"/>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
+    <row r="9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A9" s="11" t="inlineStr">
         <is>
           <t>لماكينة</t>
         </is>
       </c>
-      <c r="B9" s="13" t="inlineStr">
+      <c r="B9" s="12" t="inlineStr">
         <is>
           <t>وسيط التوالف</t>
         </is>
       </c>
       <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
+      <c r="D9" s="18" t="n"/>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="15" t="n"/>
       <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
+      <c r="D10" s="18" t="n"/>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
+    <row r="11" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="15" t="n"/>
       <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
+      <c r="D11" s="19" t="n"/>
       <c r="E11" s="9" t="n"/>
       <c r="F11" s="9" t="n"/>
     </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
+    <row r="12" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A12" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
         </is>
       </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
+      <c r="B12" s="28" t="n"/>
+      <c r="C12" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
+      <c r="D12" s="26" t="n"/>
+      <c r="E12" s="26" t="n"/>
+      <c r="F12" s="26" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="A13" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
         </is>
       </c>
-      <c r="B13" s="13" t="inlineStr">
+      <c r="B13" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
         </is>
@@ -3187,7 +3158,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D13" s="18" t="inlineStr">
+      <c r="D13" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -3203,135 +3174,123 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="37" t="n">
-        <v>5</v>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="35" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" s="36" t="n">
+        <v>3</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>LG65UP77_TB</t>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>بوتجاز  90 تصدير</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
+    <row r="15" ht="18" customHeight="1">
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="33" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
+        <v>6</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>LG 65UP77 FRONT</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="33" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t>LG43UP79</t>
+        <v>7</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D17" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
+    <row r="17" ht="18" customHeight="1">
+      <c r="A17" s="30" t="n"/>
+      <c r="B17" s="33" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D18" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="30" t="n"/>
+      <c r="B18" s="33" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="30" t="n"/>
+      <c r="B19" s="33" t="n"/>
       <c r="C19" s="4" t="n"/>
-      <c r="D19" s="19" t="n"/>
+      <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="30" t="n"/>
+      <c r="B20" s="33" t="n"/>
       <c r="C20" s="4" t="n"/>
-      <c r="D20" s="19" t="n"/>
+      <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="30" t="n"/>
+      <c r="B21" s="33" t="n"/>
       <c r="C21" s="4" t="n"/>
-      <c r="D21" s="19" t="n"/>
+      <c r="D21" s="18" t="n"/>
       <c r="E21" s="9" t="n"/>
       <c r="F21" s="9" t="n"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
+    <row r="22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A22" s="22" t="n"/>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
+      <c r="D22" s="20" t="n"/>
       <c r="E22" s="9" t="n"/>
       <c r="F22" s="9" t="n"/>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
+    <row r="23" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A23" s="27" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
         </is>
       </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
+      <c r="B23" s="28" t="n"/>
+      <c r="C23" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="D23" s="26" t="n"/>
+      <c r="E23" s="26" t="n"/>
+      <c r="F23" s="26" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
         </is>
       </c>
-      <c r="B24" s="13" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
         </is>
@@ -3341,7 +3300,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D24" s="18" t="inlineStr">
+      <c r="D24" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -3357,94 +3316,100 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n"/>
-      <c r="B25" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="19" t="n"/>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="35" t="n">
+        <v>6</v>
+      </c>
+      <c r="B25" s="36" t="n"/>
+      <c r="C25" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="30" t="n"/>
+      <c r="B26" s="33" t="n"/>
       <c r="C26" s="4" t="n"/>
-      <c r="D26" s="19" t="n"/>
+      <c r="D26" s="18" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
+    <row r="27" ht="18" customHeight="1">
+      <c r="A27" s="30" t="n"/>
+      <c r="B27" s="33" t="n"/>
       <c r="C27" s="4" t="n"/>
-      <c r="D27" s="19" t="n"/>
+      <c r="D27" s="18" t="n"/>
       <c r="E27" s="9" t="n"/>
       <c r="F27" s="9" t="n"/>
     </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
+    <row r="28" ht="18" customHeight="1">
+      <c r="A28" s="30" t="n"/>
+      <c r="B28" s="33" t="n"/>
       <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
+      <c r="D28" s="18" t="n"/>
       <c r="E28" s="9" t="n"/>
       <c r="F28" s="9" t="n"/>
     </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
+    <row r="29" ht="18" customHeight="1">
+      <c r="A29" s="30" t="n"/>
+      <c r="B29" s="33" t="n"/>
       <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
+      <c r="D29" s="18" t="n"/>
       <c r="E29" s="9" t="n"/>
       <c r="F29" s="9" t="n"/>
     </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="30" t="n"/>
+      <c r="B30" s="33" t="n"/>
       <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
+      <c r="D30" s="18" t="n"/>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="9" t="n"/>
     </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="30" t="n"/>
+      <c r="B31" s="33" t="n"/>
       <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
+      <c r="D31" s="18" t="n"/>
       <c r="E31" s="9" t="n"/>
       <c r="F31" s="9" t="n"/>
     </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
+    <row r="32" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A32" s="30" t="n"/>
+      <c r="B32" s="33" t="n"/>
       <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
+      <c r="D32" s="19" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
     </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
+    <row r="33" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A33" s="27" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
         </is>
       </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
+      <c r="B33" s="28" t="n"/>
+      <c r="C33" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
+      <c r="D33" s="26" t="n"/>
+      <c r="E33" s="26" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1">
+      <c r="A34" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
         </is>
       </c>
-      <c r="B34" s="12" t="inlineStr">
+      <c r="B34" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
         </is>
@@ -3454,7 +3419,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D34" s="18" t="inlineStr">
+      <c r="D34" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -3470,77 +3435,89 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n">
-        <v>14</v>
-      </c>
-      <c r="B35" s="33" t="n">
-        <v>1</v>
+    <row r="35" ht="18" customHeight="1">
+      <c r="A35" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="B35" s="32" t="n">
+        <v>4</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D35" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
+        <v>6</v>
+      </c>
+      <c r="D35" s="18" t="inlineStr">
+        <is>
+          <t>LG 65UP77 FRONT</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
       <c r="F35" s="9" t="n"/>
     </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n"/>
-      <c r="D36" s="19" t="n"/>
+    <row r="36" ht="18" customHeight="1">
+      <c r="A36" s="30" t="n"/>
+      <c r="B36" s="33" t="n"/>
+      <c r="C36" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D36" s="18" t="inlineStr">
+        <is>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
+        </is>
+      </c>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="19" t="n"/>
+    <row r="37" ht="18" customHeight="1">
+      <c r="A37" s="30" t="n"/>
+      <c r="B37" s="33" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="D37" s="18" t="inlineStr">
+        <is>
+          <t>فوم كوش 152</t>
+        </is>
+      </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
+    <row r="38" ht="18" customHeight="1">
+      <c r="A38" s="30" t="n"/>
+      <c r="B38" s="33" t="n"/>
       <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
+      <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
+    <row r="39" ht="18" customHeight="1">
+      <c r="A39" s="30" t="n"/>
+      <c r="B39" s="33" t="n"/>
       <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
+      <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
+    <row r="40" ht="18" customHeight="1">
+      <c r="A40" s="30" t="n"/>
+      <c r="B40" s="33" t="n"/>
       <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
+      <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
+    <row r="41" ht="18" customHeight="1">
+      <c r="A41" s="30" t="n"/>
+      <c r="B41" s="33" t="n"/>
       <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
+      <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
+    <row r="42" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A42" s="31" t="n"/>
+      <c r="B42" s="34" t="n"/>
       <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
+      <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
     </row>
@@ -3582,15 +3559,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
+    <col width="26.625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.625" customWidth="1" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="21" min="4" max="4"/>
+    <col width="28.875" customWidth="1" min="5" max="5"/>
+    <col width="31.875" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
+    <row r="1" ht="18.75" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
@@ -3598,41 +3575,41 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D1" s="17" t="n">
-        <v>2022</v>
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="n">
+        <v>2023</v>
       </c>
       <c r="E1" s="3" t="n"/>
       <c r="F1" s="3" t="n"/>
     </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
+    <row r="2" ht="21" customHeight="1" thickBot="1">
+      <c r="A2" s="37" t="inlineStr">
         <is>
           <t>اولا : نسبة التالف على الماكينات</t>
         </is>
       </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
+      <c r="B2" s="28" t="n"/>
+      <c r="C2" s="23" t="inlineStr">
         <is>
           <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
         </is>
       </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="D2" s="24" t="n"/>
+      <c r="E2" s="24" t="n"/>
+      <c r="F2" s="24" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
         </is>
@@ -3642,7 +3619,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D3" s="18" t="inlineStr">
+      <c r="D3" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -3658,137 +3635,125 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n">
-        <v>0.8631486308093288</v>
-      </c>
-      <c r="B4" s="40" t="n">
-        <v>0.8631207917212707</v>
+    <row r="4" ht="21.75" customHeight="1">
+      <c r="A4" s="38" t="n">
+        <v>0.7400714254980423</v>
+      </c>
+      <c r="B4" s="39" t="n">
+        <v>0.9533839587606008</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>LG65UP77_TB</t>
+        <v>5</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
     </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
+    <row r="5" ht="21.75" customHeight="1">
+      <c r="A5" s="30" t="n"/>
+      <c r="B5" s="33" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" s="19" t="inlineStr">
-        <is>
-          <t>LG43UP79</t>
+        <v>8</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
+    <row r="6" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>لماكينة</t>
         </is>
       </c>
-      <c r="B6" s="13" t="inlineStr">
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>70UQ80006LD</t>
-        </is>
-      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="18" t="n"/>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D7" s="19" t="inlineStr">
-        <is>
-          <t>زانوسي العبد 303-304-308-314</t>
-        </is>
-      </c>
+    <row r="7" ht="21.75" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="15" t="n"/>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="18" t="n"/>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
+    <row r="8" ht="21.75" customHeight="1">
+      <c r="A8" s="13" t="n"/>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="4" t="n"/>
-      <c r="D8" s="19" t="n"/>
+      <c r="D8" s="18" t="n"/>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
+    <row r="9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A9" s="11" t="inlineStr">
         <is>
           <t>لماكينة</t>
         </is>
       </c>
-      <c r="B9" s="13" t="inlineStr">
+      <c r="B9" s="12" t="inlineStr">
         <is>
           <t>وسيط التوالف</t>
         </is>
       </c>
       <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
+      <c r="D9" s="18" t="n"/>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="15" t="n"/>
       <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
+      <c r="D10" s="18" t="n"/>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
+    <row r="11" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="15" t="n"/>
       <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
+      <c r="D11" s="19" t="n"/>
       <c r="E11" s="9" t="n"/>
       <c r="F11" s="9" t="n"/>
     </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
+    <row r="12" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A12" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
         </is>
       </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
+      <c r="B12" s="28" t="n"/>
+      <c r="C12" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
+      <c r="D12" s="26" t="n"/>
+      <c r="E12" s="26" t="n"/>
+      <c r="F12" s="26" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="A13" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
         </is>
       </c>
-      <c r="B13" s="13" t="inlineStr">
+      <c r="B13" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
         </is>
@@ -3798,7 +3763,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D13" s="18" t="inlineStr">
+      <c r="D13" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -3814,31 +3779,31 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n">
-        <v>11</v>
-      </c>
-      <c r="B14" s="37" t="n">
-        <v>5</v>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="35" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="36" t="n">
+        <v>2</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>LG65UP77_TB</t>
+        <v>6</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>LG 65UP77 FRONT</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
+    <row r="15" ht="18" customHeight="1">
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="33" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" s="19" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
         <is>
           <t>طقم سخان نبتون ذو 3 اطقم</t>
         </is>
@@ -3846,103 +3811,85 @@
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="C16" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t>LG43UP79</t>
-        </is>
-      </c>
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="33" t="n"/>
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="18" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D17" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
+    <row r="17" ht="18" customHeight="1">
+      <c r="A17" s="30" t="n"/>
+      <c r="B17" s="33" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D18" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="30" t="n"/>
+      <c r="B18" s="33" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="30" t="n"/>
+      <c r="B19" s="33" t="n"/>
       <c r="C19" s="4" t="n"/>
-      <c r="D19" s="19" t="n"/>
+      <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="30" t="n"/>
+      <c r="B20" s="33" t="n"/>
       <c r="C20" s="4" t="n"/>
-      <c r="D20" s="19" t="n"/>
+      <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="30" t="n"/>
+      <c r="B21" s="33" t="n"/>
       <c r="C21" s="4" t="n"/>
-      <c r="D21" s="19" t="n"/>
+      <c r="D21" s="18" t="n"/>
       <c r="E21" s="9" t="n"/>
       <c r="F21" s="9" t="n"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
+    <row r="22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A22" s="22" t="n"/>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
+      <c r="D22" s="20" t="n"/>
       <c r="E22" s="9" t="n"/>
       <c r="F22" s="9" t="n"/>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
+    <row r="23" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A23" s="27" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
         </is>
       </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
+      <c r="B23" s="28" t="n"/>
+      <c r="C23" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="D23" s="26" t="n"/>
+      <c r="E23" s="26" t="n"/>
+      <c r="F23" s="26" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
         </is>
       </c>
-      <c r="B24" s="13" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
         </is>
@@ -3952,7 +3899,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D24" s="18" t="inlineStr">
+      <c r="D24" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -3968,94 +3915,108 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n"/>
-      <c r="B25" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="19" t="n"/>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="35" t="n">
+        <v>7</v>
+      </c>
+      <c r="B25" s="36" t="n">
+        <v/>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
+        </is>
+      </c>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="19" t="n"/>
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="30" t="n"/>
+      <c r="B26" s="33" t="n"/>
+      <c r="C26" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D26" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
+    <row r="27" ht="18" customHeight="1">
+      <c r="A27" s="30" t="n"/>
+      <c r="B27" s="33" t="n"/>
       <c r="C27" s="4" t="n"/>
-      <c r="D27" s="19" t="n"/>
+      <c r="D27" s="18" t="n"/>
       <c r="E27" s="9" t="n"/>
       <c r="F27" s="9" t="n"/>
     </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
+    <row r="28" ht="18" customHeight="1">
+      <c r="A28" s="30" t="n"/>
+      <c r="B28" s="33" t="n"/>
       <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
+      <c r="D28" s="18" t="n"/>
       <c r="E28" s="9" t="n"/>
       <c r="F28" s="9" t="n"/>
     </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
+    <row r="29" ht="18" customHeight="1">
+      <c r="A29" s="30" t="n"/>
+      <c r="B29" s="33" t="n"/>
       <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
+      <c r="D29" s="18" t="n"/>
       <c r="E29" s="9" t="n"/>
       <c r="F29" s="9" t="n"/>
     </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="30" t="n"/>
+      <c r="B30" s="33" t="n"/>
       <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
+      <c r="D30" s="18" t="n"/>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="9" t="n"/>
     </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="30" t="n"/>
+      <c r="B31" s="33" t="n"/>
       <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
+      <c r="D31" s="18" t="n"/>
       <c r="E31" s="9" t="n"/>
       <c r="F31" s="9" t="n"/>
     </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
+    <row r="32" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A32" s="30" t="n"/>
+      <c r="B32" s="33" t="n"/>
       <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
+      <c r="D32" s="19" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
     </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
+    <row r="33" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A33" s="27" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
         </is>
       </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
+      <c r="B33" s="28" t="n"/>
+      <c r="C33" s="25" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
+      <c r="D33" s="26" t="n"/>
+      <c r="E33" s="26" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1">
+      <c r="A34" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
         </is>
       </c>
-      <c r="B34" s="12" t="inlineStr">
+      <c r="B34" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
         </is>
@@ -4065,7 +4026,7 @@
           <t>رقم الماكينة</t>
         </is>
       </c>
-      <c r="D34" s="18" t="inlineStr">
+      <c r="D34" s="17" t="inlineStr">
         <is>
           <t>الصنف الغير مطابق</t>
         </is>
@@ -4081,1277 +4042,89 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n">
-        <v>15</v>
-      </c>
-      <c r="B35" s="33" t="n">
-        <v>1</v>
+    <row r="35" ht="18" customHeight="1">
+      <c r="A35" s="29" t="n">
+        <v>7</v>
+      </c>
+      <c r="B35" s="32" t="n">
+        <v>5</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D35" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
+        <v>4</v>
+      </c>
+      <c r="D35" s="18" t="inlineStr">
+        <is>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
       <c r="F35" s="9" t="n"/>
     </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n"/>
-      <c r="D36" s="19" t="n"/>
+    <row r="36" ht="18" customHeight="1">
+      <c r="A36" s="30" t="n"/>
+      <c r="B36" s="33" t="n"/>
+      <c r="C36" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D36" s="18" t="inlineStr">
+        <is>
+          <t>LG 65UP77 FRONT</t>
+        </is>
+      </c>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="19" t="n"/>
+    <row r="37" ht="18" customHeight="1">
+      <c r="A37" s="30" t="n"/>
+      <c r="B37" s="33" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D37" s="18" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
+    <row r="38" ht="18" customHeight="1">
+      <c r="A38" s="30" t="n"/>
+      <c r="B38" s="33" t="n"/>
       <c r="C38" s="4" t="n"/>
-      <c r="D38" s="19" t="n"/>
+      <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
+    <row r="39" ht="18" customHeight="1">
+      <c r="A39" s="30" t="n"/>
+      <c r="B39" s="33" t="n"/>
       <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
+      <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
+    <row r="40" ht="18" customHeight="1">
+      <c r="A40" s="30" t="n"/>
+      <c r="B40" s="33" t="n"/>
       <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
+      <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
+    <row r="41" ht="18" customHeight="1">
+      <c r="A41" s="30" t="n"/>
+      <c r="B41" s="33" t="n"/>
       <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
+      <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
+    <row r="42" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A42" s="31" t="n"/>
+      <c r="B42" s="34" t="n"/>
       <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
-      <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
-  <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D1" s="17" t="n">
-        <v>2022</v>
-      </c>
-      <c r="E1" s="3" t="n"/>
-      <c r="F1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
-        <is>
-          <t>اولا : نسبة التالف على الماكينات</t>
-        </is>
-      </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
-        <is>
-          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
-        </is>
-      </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
-        </is>
-      </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E3" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n">
-        <v>0.7745091378490386</v>
-      </c>
-      <c r="B4" s="40" t="n">
-        <v>0.6802721088435374</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>فوم طقم سخان غاز 10 لتر</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="n"/>
-      <c r="F4" s="9" t="n"/>
-    </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
-      <c r="C5" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D5" s="19" t="inlineStr">
-        <is>
-          <t>فوم قاعده 60*60</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="n"/>
-      <c r="F5" s="9" t="n"/>
-    </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>اعلي نسبة توالف</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="19" t="n"/>
-      <c r="E6" s="9" t="n"/>
-      <c r="F6" s="9" t="n"/>
-    </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="19" t="n"/>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-    </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="19" t="n"/>
-      <c r="E8" s="9" t="n"/>
-      <c r="F8" s="9" t="n"/>
-    </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B9" s="13" t="inlineStr">
-        <is>
-          <t>وسيط التوالف</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
-      <c r="E9" s="9" t="n"/>
-      <c r="F9" s="9" t="n"/>
-    </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
-      <c r="E10" s="9" t="n"/>
-      <c r="F10" s="9" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
-      <c r="E11" s="9" t="n"/>
-      <c r="F11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
-        </is>
-      </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
-        </is>
-      </c>
-      <c r="B13" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D13" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n">
-        <v>11</v>
-      </c>
-      <c r="B14" s="37" t="n">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>oled55cs6la</t>
-        </is>
-      </c>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-    </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
-      <c r="C15" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D15" s="19" t="inlineStr">
-        <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
-        </is>
-      </c>
-      <c r="E15" s="9" t="n"/>
-      <c r="F15" s="9" t="n"/>
-    </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="C16" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t>زانوسي 70 سم -2 (قاعدة ، كفر)</t>
-        </is>
-      </c>
-      <c r="E16" s="9" t="n"/>
-      <c r="F16" s="9" t="n"/>
-    </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D17" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
-      <c r="E17" s="9" t="n"/>
-      <c r="F17" s="9" t="n"/>
-    </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="19" t="n"/>
-      <c r="E18" s="9" t="n"/>
-      <c r="F18" s="9" t="n"/>
-    </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="19" t="n"/>
-      <c r="E19" s="9" t="n"/>
-      <c r="F19" s="9" t="n"/>
-    </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="19" t="n"/>
-      <c r="E20" s="9" t="n"/>
-      <c r="F20" s="9" t="n"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="19" t="n"/>
-      <c r="E21" s="9" t="n"/>
-      <c r="F21" s="9" t="n"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
-      <c r="E22" s="9" t="n"/>
-      <c r="F22" s="9" t="n"/>
-    </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
-        </is>
-      </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B24" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
-        </is>
-      </c>
-      <c r="C24" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D24" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E24" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F24" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n">
-        <v>11</v>
-      </c>
-      <c r="B25" s="37" t="n"/>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="19" t="n"/>
-      <c r="E25" s="9" t="n"/>
-      <c r="F25" s="9" t="n"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="19" t="n"/>
-      <c r="E26" s="9" t="n"/>
-      <c r="F26" s="9" t="n"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="19" t="n"/>
-      <c r="E27" s="9" t="n"/>
-      <c r="F27" s="9" t="n"/>
-    </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
-      <c r="E28" s="9" t="n"/>
-      <c r="F28" s="9" t="n"/>
-    </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
-      <c r="E29" s="9" t="n"/>
-      <c r="F29" s="9" t="n"/>
-    </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
-      <c r="E30" s="9" t="n"/>
-      <c r="F30" s="9" t="n"/>
-    </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
-      <c r="E31" s="9" t="n"/>
-      <c r="F31" s="9" t="n"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
-      <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
-      <c r="E32" s="10" t="n"/>
-      <c r="F32" s="10" t="n"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
-        </is>
-      </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
-        </is>
-      </c>
-      <c r="C34" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D34" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E34" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F34" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n">
-        <v>11</v>
-      </c>
-      <c r="B35" s="33" t="n">
-        <v>4</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="19" t="inlineStr">
-        <is>
-          <t>LG43LM63-UM73</t>
-        </is>
-      </c>
-      <c r="E35" s="9" t="n"/>
-      <c r="F35" s="9" t="n"/>
-    </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D36" s="19" t="inlineStr">
-        <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
-        </is>
-      </c>
-      <c r="E36" s="9" t="n"/>
-      <c r="F36" s="9" t="n"/>
-    </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D37" s="19" t="inlineStr">
-        <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
-        </is>
-      </c>
-      <c r="E37" s="9" t="n"/>
-      <c r="F37" s="9" t="n"/>
-    </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
-      <c r="C38" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="D38" s="19" t="inlineStr">
-        <is>
-          <t>فوم طقم سخان غاز 10 لتر</t>
-        </is>
-      </c>
-      <c r="E38" s="9" t="n"/>
-      <c r="F38" s="9" t="n"/>
-    </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
-      <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
-      <c r="E39" s="9" t="n"/>
-      <c r="F39" s="9" t="n"/>
-    </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
-      <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
-      <c r="E40" s="9" t="n"/>
-      <c r="F40" s="9" t="n"/>
-    </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
-      <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
-      <c r="E41" s="9" t="n"/>
-      <c r="F41" s="9" t="n"/>
-    </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
-      <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
-      <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
-  <cols>
-    <col width="26.625" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
-    <col width="31.25" bestFit="1" customWidth="1" style="11" min="2" max="2"/>
-    <col width="10.625" customWidth="1" style="11" min="3" max="3"/>
-    <col width="20.125" customWidth="1" style="22" min="4" max="4"/>
-    <col width="28.875" customWidth="1" style="11" min="5" max="5"/>
-    <col width="31.875" customWidth="1" style="11" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="17" t="n">
-        <v>2022</v>
-      </c>
-      <c r="E1" s="3" t="n"/>
-      <c r="F1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="21" customHeight="1" s="11" thickBot="1">
-      <c r="A2" s="38" t="inlineStr">
-        <is>
-          <t>اولا : نسبة التالف على الماكينات</t>
-        </is>
-      </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="24" t="inlineStr">
-        <is>
-          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
-        </is>
-      </c>
-      <c r="D2" s="25" t="n"/>
-      <c r="E2" s="25" t="n"/>
-      <c r="F2" s="25" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
-        </is>
-      </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E3" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="21.75" customHeight="1" s="11">
-      <c r="A4" s="39" t="n">
-        <v>101.010101010101</v>
-      </c>
-      <c r="B4" s="40" t="n">
-        <v>101.2345679012346</v>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="19" t="n"/>
-      <c r="E4" s="9" t="n"/>
-      <c r="F4" s="9" t="n"/>
-    </row>
-    <row r="5" ht="21.75" customHeight="1" s="11">
-      <c r="A5" s="31" t="n"/>
-      <c r="B5" s="34" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="19" t="n"/>
-      <c r="E5" s="9" t="n"/>
-      <c r="F5" s="9" t="n"/>
-    </row>
-    <row r="6" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>اعلي نسبة توالف</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="19" t="n"/>
-      <c r="E6" s="9" t="n"/>
-      <c r="F6" s="9" t="n"/>
-    </row>
-    <row r="7" ht="21.75" customHeight="1" s="11">
-      <c r="A7" s="14" t="n"/>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="19" t="n"/>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-    </row>
-    <row r="8" ht="21.75" customHeight="1" s="11">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="19" t="n"/>
-      <c r="E8" s="9" t="n"/>
-      <c r="F8" s="9" t="n"/>
-    </row>
-    <row r="9" ht="21.75" customHeight="1" s="11" thickBot="1">
-      <c r="A9" s="12" t="inlineStr">
-        <is>
-          <t>لماكينة</t>
-        </is>
-      </c>
-      <c r="B9" s="13" t="inlineStr">
-        <is>
-          <t>وسيط التوالف</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="19" t="n"/>
-      <c r="E9" s="9" t="n"/>
-      <c r="F9" s="9" t="n"/>
-    </row>
-    <row r="10" ht="18" customHeight="1" s="11">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="16" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="19" t="n"/>
-      <c r="E10" s="9" t="n"/>
-      <c r="F10" s="9" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="5" t="n"/>
-      <c r="D11" s="20" t="n"/>
-      <c r="E11" s="9" t="n"/>
-      <c r="F11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A12" s="28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
-        </is>
-      </c>
-      <c r="B12" s="29" t="n"/>
-      <c r="C12" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A13" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
-        </is>
-      </c>
-      <c r="B13" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D13" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="18" customHeight="1" s="11">
-      <c r="A14" s="36" t="n">
-        <v>6</v>
-      </c>
-      <c r="B14" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-    </row>
-    <row r="15" ht="18" customHeight="1" s="11">
-      <c r="A15" s="31" t="n"/>
-      <c r="B15" s="34" t="n"/>
-      <c r="C15" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" s="19" t="inlineStr">
-        <is>
-          <t>صندوق سمك 25 ك</t>
-        </is>
-      </c>
-      <c r="E15" s="9" t="n"/>
-      <c r="F15" s="9" t="n"/>
-    </row>
-    <row r="16" ht="18" customHeight="1" s="11">
-      <c r="A16" s="31" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="19" t="n"/>
-      <c r="E16" s="9" t="n"/>
-      <c r="F16" s="9" t="n"/>
-    </row>
-    <row r="17" ht="18" customHeight="1" s="11">
-      <c r="A17" s="31" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="19" t="n"/>
-      <c r="E17" s="9" t="n"/>
-      <c r="F17" s="9" t="n"/>
-    </row>
-    <row r="18" ht="18" customHeight="1" s="11">
-      <c r="A18" s="31" t="n"/>
-      <c r="B18" s="34" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="19" t="n"/>
-      <c r="E18" s="9" t="n"/>
-      <c r="F18" s="9" t="n"/>
-    </row>
-    <row r="19" ht="18" customHeight="1" s="11">
-      <c r="A19" s="31" t="n"/>
-      <c r="B19" s="34" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="19" t="n"/>
-      <c r="E19" s="9" t="n"/>
-      <c r="F19" s="9" t="n"/>
-    </row>
-    <row r="20" ht="18" customHeight="1" s="11">
-      <c r="A20" s="31" t="n"/>
-      <c r="B20" s="34" t="n"/>
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="19" t="n"/>
-      <c r="E20" s="9" t="n"/>
-      <c r="F20" s="9" t="n"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" s="11">
-      <c r="A21" s="31" t="n"/>
-      <c r="B21" s="34" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="19" t="n"/>
-      <c r="E21" s="9" t="n"/>
-      <c r="F21" s="9" t="n"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" s="11" thickBot="1">
-      <c r="A22" s="23" t="n"/>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="21" t="n"/>
-      <c r="E22" s="9" t="n"/>
-      <c r="F22" s="9" t="n"/>
-    </row>
-    <row r="23" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A23" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
-        </is>
-      </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A24" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B24" s="13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
-        </is>
-      </c>
-      <c r="C24" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D24" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E24" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F24" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="18" customHeight="1" s="11">
-      <c r="A25" s="36" t="n">
-        <v>4</v>
-      </c>
-      <c r="B25" s="37" t="n">
-        <v/>
-      </c>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="19" t="n"/>
-      <c r="E25" s="9" t="n"/>
-      <c r="F25" s="9" t="n"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" s="11">
-      <c r="A26" s="31" t="n"/>
-      <c r="B26" s="34" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="19" t="n"/>
-      <c r="E26" s="9" t="n"/>
-      <c r="F26" s="9" t="n"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" s="11">
-      <c r="A27" s="31" t="n"/>
-      <c r="B27" s="34" t="n"/>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="19" t="n"/>
-      <c r="E27" s="9" t="n"/>
-      <c r="F27" s="9" t="n"/>
-    </row>
-    <row r="28" ht="18" customHeight="1" s="11">
-      <c r="A28" s="31" t="n"/>
-      <c r="B28" s="34" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="19" t="n"/>
-      <c r="E28" s="9" t="n"/>
-      <c r="F28" s="9" t="n"/>
-    </row>
-    <row r="29" ht="18" customHeight="1" s="11">
-      <c r="A29" s="31" t="n"/>
-      <c r="B29" s="34" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="19" t="n"/>
-      <c r="E29" s="9" t="n"/>
-      <c r="F29" s="9" t="n"/>
-    </row>
-    <row r="30" ht="18" customHeight="1" s="11">
-      <c r="A30" s="31" t="n"/>
-      <c r="B30" s="34" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="19" t="n"/>
-      <c r="E30" s="9" t="n"/>
-      <c r="F30" s="9" t="n"/>
-    </row>
-    <row r="31" ht="18" customHeight="1" s="11">
-      <c r="A31" s="31" t="n"/>
-      <c r="B31" s="34" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="19" t="n"/>
-      <c r="E31" s="9" t="n"/>
-      <c r="F31" s="9" t="n"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A32" s="31" t="n"/>
-      <c r="B32" s="34" t="n"/>
-      <c r="C32" s="5" t="n"/>
-      <c r="D32" s="20" t="n"/>
-      <c r="E32" s="10" t="n"/>
-      <c r="F32" s="10" t="n"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A33" s="28" t="inlineStr">
-        <is>
-          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
-        </is>
-      </c>
-      <c r="B33" s="29" t="n"/>
-      <c r="C33" s="26" t="inlineStr">
-        <is>
-          <t>ملاحظات</t>
-        </is>
-      </c>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
-    </row>
-    <row r="34" ht="18" customHeight="1" s="11" thickBot="1">
-      <c r="A34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
-        </is>
-      </c>
-      <c r="B34" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
-        </is>
-      </c>
-      <c r="C34" s="7" t="inlineStr">
-        <is>
-          <t>رقم الماكينة</t>
-        </is>
-      </c>
-      <c r="D34" s="18" t="inlineStr">
-        <is>
-          <t>الصنف الغير مطابق</t>
-        </is>
-      </c>
-      <c r="E34" s="8" t="inlineStr">
-        <is>
-          <t>السبب</t>
-        </is>
-      </c>
-      <c r="F34" s="8" t="inlineStr">
-        <is>
-          <t>الاجراء التصحيحي لمعالجة السبب</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="18" customHeight="1" s="11">
-      <c r="A35" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="B35" s="33" t="n">
-        <v>4</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D35" s="19" t="inlineStr">
-        <is>
-          <t>زانوسى العبد 305</t>
-        </is>
-      </c>
-      <c r="E35" s="9" t="n"/>
-      <c r="F35" s="9" t="n"/>
-    </row>
-    <row r="36" ht="18" customHeight="1" s="11">
-      <c r="A36" s="31" t="n"/>
-      <c r="B36" s="34" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D36" s="19" t="inlineStr">
-        <is>
-          <t>LG65UM73</t>
-        </is>
-      </c>
-      <c r="E36" s="9" t="n"/>
-      <c r="F36" s="9" t="n"/>
-    </row>
-    <row r="37" ht="18" customHeight="1" s="11">
-      <c r="A37" s="31" t="n"/>
-      <c r="B37" s="34" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D37" s="19" t="inlineStr">
-        <is>
-          <t>LG43LM63-UM73</t>
-        </is>
-      </c>
-      <c r="E37" s="9" t="n"/>
-      <c r="F37" s="9" t="n"/>
-    </row>
-    <row r="38" ht="18" customHeight="1" s="11">
-      <c r="A38" s="31" t="n"/>
-      <c r="B38" s="34" t="n"/>
-      <c r="C38" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D38" s="19" t="inlineStr">
-        <is>
-          <t>طقم سخان بلونايل ذو 4 اطقم</t>
-        </is>
-      </c>
-      <c r="E38" s="9" t="n"/>
-      <c r="F38" s="9" t="n"/>
-    </row>
-    <row r="39" ht="18" customHeight="1" s="11">
-      <c r="A39" s="31" t="n"/>
-      <c r="B39" s="34" t="n"/>
-      <c r="C39" s="4" t="n"/>
-      <c r="D39" s="19" t="n"/>
-      <c r="E39" s="9" t="n"/>
-      <c r="F39" s="9" t="n"/>
-    </row>
-    <row r="40" ht="18" customHeight="1" s="11">
-      <c r="A40" s="31" t="n"/>
-      <c r="B40" s="34" t="n"/>
-      <c r="C40" s="4" t="n"/>
-      <c r="D40" s="19" t="n"/>
-      <c r="E40" s="9" t="n"/>
-      <c r="F40" s="9" t="n"/>
-    </row>
-    <row r="41" ht="18" customHeight="1" s="11">
-      <c r="A41" s="31" t="n"/>
-      <c r="B41" s="34" t="n"/>
-      <c r="C41" s="4" t="n"/>
-      <c r="D41" s="19" t="n"/>
-      <c r="E41" s="9" t="n"/>
-      <c r="F41" s="9" t="n"/>
-    </row>
-    <row r="42" ht="18.75" customHeight="1" s="11" thickBot="1">
-      <c r="A42" s="32" t="n"/>
-      <c r="B42" s="35" t="n"/>
-      <c r="C42" s="5" t="n"/>
-      <c r="D42" s="20" t="n"/>
+      <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
     </row>

</xml_diff>

<commit_message>
restrucure code to get yearl yeport based on daily and montly report code
</commit_message>
<xml_diff>
--- a/apps/analysis/formats/QC_molds_daily_summary.xlsx
+++ b/apps/analysis/formats/QC_molds_daily_summary.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="10" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="AccessDatabase" hidden="1">"C:\Documents and Settings\Administrator\My Documents\BITUNIL\FINANCE\SAMEER\Cost StudyHB.mdb"</definedName>
@@ -43,7 +44,7 @@
     <definedName name="الاوزان">'[5]0'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'daily'!$A$2:$F$2</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -436,15 +437,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -461,6 +453,15 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -529,18 +530,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -560,12 +549,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="2" fontId="7" fillId="5" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="5" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1841,20 +1842,20 @@
       <c r="F1" s="3" t="n"/>
     </row>
     <row r="2" ht="21" customHeight="1" thickBot="1">
-      <c r="A2" s="37" t="inlineStr">
+      <c r="A2" s="31" t="inlineStr">
         <is>
           <t>اولا : نسبة التالف على الماكينات</t>
         </is>
       </c>
-      <c r="B2" s="28" t="n"/>
-      <c r="C2" s="23" t="inlineStr">
+      <c r="B2" s="32" t="n"/>
+      <c r="C2" s="36" t="inlineStr">
         <is>
           <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
         </is>
       </c>
-      <c r="D2" s="24" t="n"/>
-      <c r="E2" s="24" t="n"/>
-      <c r="F2" s="24" t="n"/>
+      <c r="D2" s="37" t="n"/>
+      <c r="E2" s="37" t="n"/>
+      <c r="F2" s="37" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1" thickBot="1">
       <c r="A3" s="11" t="inlineStr">
@@ -1889,16 +1890,16 @@
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="38" t="n"/>
-      <c r="B4" s="39" t="n"/>
+      <c r="A4" s="34" t="n"/>
+      <c r="B4" s="35" t="n"/>
       <c r="C4" s="4" t="n"/>
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
     </row>
     <row r="5" ht="21.75" customHeight="1">
-      <c r="A5" s="30" t="n"/>
-      <c r="B5" s="33" t="n"/>
+      <c r="A5" s="24" t="n"/>
+      <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="18" t="n"/>
       <c r="E5" s="9" t="n"/>
@@ -1969,20 +1970,20 @@
       <c r="F11" s="9" t="n"/>
     </row>
     <row r="12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A12" s="27" t="inlineStr">
+      <c r="A12" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
         </is>
       </c>
-      <c r="B12" s="28" t="n"/>
-      <c r="C12" s="25" t="inlineStr">
+      <c r="B12" s="32" t="n"/>
+      <c r="C12" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D12" s="26" t="n"/>
-      <c r="E12" s="26" t="n"/>
-      <c r="F12" s="26" t="n"/>
+      <c r="D12" s="39" t="n"/>
+      <c r="E12" s="39" t="n"/>
+      <c r="F12" s="39" t="n"/>
     </row>
     <row r="13" ht="18" customHeight="1" thickBot="1">
       <c r="A13" s="11" t="inlineStr">
@@ -2017,64 +2018,64 @@
       </c>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="A14" s="35" t="n"/>
-      <c r="B14" s="36" t="n"/>
+      <c r="A14" s="29" t="n"/>
+      <c r="B14" s="30" t="n"/>
       <c r="C14" s="4" t="n"/>
       <c r="D14" s="18" t="n"/>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
-      <c r="A15" s="30" t="n"/>
-      <c r="B15" s="33" t="n"/>
+      <c r="A15" s="24" t="n"/>
+      <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n"/>
       <c r="D15" s="18" t="n"/>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
-      <c r="A16" s="30" t="n"/>
-      <c r="B16" s="33" t="n"/>
+      <c r="A16" s="24" t="n"/>
+      <c r="B16" s="27" t="n"/>
       <c r="C16" s="4" t="n"/>
       <c r="D16" s="18" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
-      <c r="A17" s="30" t="n"/>
-      <c r="B17" s="33" t="n"/>
+      <c r="A17" s="24" t="n"/>
+      <c r="B17" s="27" t="n"/>
       <c r="C17" s="4" t="n"/>
       <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="30" t="n"/>
-      <c r="B18" s="33" t="n"/>
+      <c r="A18" s="24" t="n"/>
+      <c r="B18" s="27" t="n"/>
       <c r="C18" s="4" t="n"/>
       <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="30" t="n"/>
-      <c r="B19" s="33" t="n"/>
+      <c r="A19" s="24" t="n"/>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
     <row r="20" ht="18" customHeight="1">
-      <c r="A20" s="30" t="n"/>
-      <c r="B20" s="33" t="n"/>
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="27" t="n"/>
       <c r="C20" s="4" t="n"/>
       <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
     <row r="21" ht="18" customHeight="1">
-      <c r="A21" s="30" t="n"/>
-      <c r="B21" s="33" t="n"/>
+      <c r="A21" s="24" t="n"/>
+      <c r="B21" s="27" t="n"/>
       <c r="C21" s="4" t="n"/>
       <c r="D21" s="18" t="n"/>
       <c r="E21" s="9" t="n"/>
@@ -2089,20 +2090,20 @@
       <c r="F22" s="9" t="n"/>
     </row>
     <row r="23" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A23" s="27" t="inlineStr">
+      <c r="A23" s="33" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
         </is>
       </c>
-      <c r="B23" s="28" t="n"/>
-      <c r="C23" s="25" t="inlineStr">
+      <c r="B23" s="32" t="n"/>
+      <c r="C23" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D23" s="26" t="n"/>
-      <c r="E23" s="26" t="n"/>
-      <c r="F23" s="26" t="n"/>
+      <c r="D23" s="39" t="n"/>
+      <c r="E23" s="39" t="n"/>
+      <c r="F23" s="39" t="n"/>
     </row>
     <row r="24" ht="18" customHeight="1" thickBot="1">
       <c r="A24" s="11" t="inlineStr">
@@ -2137,83 +2138,83 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="35" t="n"/>
-      <c r="B25" s="36" t="n"/>
+      <c r="A25" s="29" t="n"/>
+      <c r="B25" s="30" t="n"/>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
     <row r="26" ht="18" customHeight="1">
-      <c r="A26" s="30" t="n"/>
-      <c r="B26" s="33" t="n"/>
+      <c r="A26" s="24" t="n"/>
+      <c r="B26" s="27" t="n"/>
       <c r="C26" s="4" t="n"/>
       <c r="D26" s="18" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
     <row r="27" ht="18" customHeight="1">
-      <c r="A27" s="30" t="n"/>
-      <c r="B27" s="33" t="n"/>
+      <c r="A27" s="24" t="n"/>
+      <c r="B27" s="27" t="n"/>
       <c r="C27" s="4" t="n"/>
       <c r="D27" s="18" t="n"/>
       <c r="E27" s="9" t="n"/>
       <c r="F27" s="9" t="n"/>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="A28" s="30" t="n"/>
-      <c r="B28" s="33" t="n"/>
+      <c r="A28" s="24" t="n"/>
+      <c r="B28" s="27" t="n"/>
       <c r="C28" s="4" t="n"/>
       <c r="D28" s="18" t="n"/>
       <c r="E28" s="9" t="n"/>
       <c r="F28" s="9" t="n"/>
     </row>
     <row r="29" ht="18" customHeight="1">
-      <c r="A29" s="30" t="n"/>
-      <c r="B29" s="33" t="n"/>
+      <c r="A29" s="24" t="n"/>
+      <c r="B29" s="27" t="n"/>
       <c r="C29" s="4" t="n"/>
       <c r="D29" s="18" t="n"/>
       <c r="E29" s="9" t="n"/>
       <c r="F29" s="9" t="n"/>
     </row>
     <row r="30" ht="18" customHeight="1">
-      <c r="A30" s="30" t="n"/>
-      <c r="B30" s="33" t="n"/>
+      <c r="A30" s="24" t="n"/>
+      <c r="B30" s="27" t="n"/>
       <c r="C30" s="4" t="n"/>
       <c r="D30" s="18" t="n"/>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="9" t="n"/>
     </row>
     <row r="31" ht="18" customHeight="1">
-      <c r="A31" s="30" t="n"/>
-      <c r="B31" s="33" t="n"/>
+      <c r="A31" s="24" t="n"/>
+      <c r="B31" s="27" t="n"/>
       <c r="C31" s="4" t="n"/>
       <c r="D31" s="18" t="n"/>
       <c r="E31" s="9" t="n"/>
       <c r="F31" s="9" t="n"/>
     </row>
     <row r="32" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A32" s="30" t="n"/>
-      <c r="B32" s="33" t="n"/>
+      <c r="A32" s="24" t="n"/>
+      <c r="B32" s="27" t="n"/>
       <c r="C32" s="5" t="n"/>
       <c r="D32" s="19" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
     </row>
     <row r="33" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A33" s="27" t="inlineStr">
+      <c r="A33" s="33" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
         </is>
       </c>
-      <c r="B33" s="28" t="n"/>
-      <c r="C33" s="25" t="inlineStr">
+      <c r="B33" s="32" t="n"/>
+      <c r="C33" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D33" s="26" t="n"/>
-      <c r="E33" s="26" t="n"/>
+      <c r="D33" s="39" t="n"/>
+      <c r="E33" s="39" t="n"/>
     </row>
     <row r="34" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="11" t="inlineStr">
@@ -2248,64 +2249,64 @@
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" s="29" t="n"/>
-      <c r="B35" s="32" t="n"/>
+      <c r="A35" s="23" t="n"/>
+      <c r="B35" s="26" t="n"/>
       <c r="C35" s="4" t="n"/>
       <c r="D35" s="18" t="n"/>
       <c r="E35" s="9" t="n"/>
       <c r="F35" s="9" t="n"/>
     </row>
     <row r="36" ht="18" customHeight="1">
-      <c r="A36" s="30" t="n"/>
-      <c r="B36" s="33" t="n"/>
+      <c r="A36" s="24" t="n"/>
+      <c r="B36" s="27" t="n"/>
       <c r="C36" s="4" t="n"/>
       <c r="D36" s="18" t="n"/>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
-      <c r="A37" s="30" t="n"/>
-      <c r="B37" s="33" t="n"/>
+      <c r="A37" s="24" t="n"/>
+      <c r="B37" s="27" t="n"/>
       <c r="C37" s="4" t="n"/>
       <c r="D37" s="18" t="n"/>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1">
-      <c r="A38" s="30" t="n"/>
-      <c r="B38" s="33" t="n"/>
+      <c r="A38" s="24" t="n"/>
+      <c r="B38" s="27" t="n"/>
       <c r="C38" s="4" t="n"/>
       <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
     <row r="39" ht="18" customHeight="1">
-      <c r="A39" s="30" t="n"/>
-      <c r="B39" s="33" t="n"/>
+      <c r="A39" s="24" t="n"/>
+      <c r="B39" s="27" t="n"/>
       <c r="C39" s="4" t="n"/>
       <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
     <row r="40" ht="18" customHeight="1">
-      <c r="A40" s="30" t="n"/>
-      <c r="B40" s="33" t="n"/>
+      <c r="A40" s="24" t="n"/>
+      <c r="B40" s="27" t="n"/>
       <c r="C40" s="4" t="n"/>
       <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="A41" s="30" t="n"/>
-      <c r="B41" s="33" t="n"/>
+      <c r="A41" s="24" t="n"/>
+      <c r="B41" s="27" t="n"/>
       <c r="C41" s="4" t="n"/>
       <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
     <row r="42" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A42" s="31" t="n"/>
-      <c r="B42" s="34" t="n"/>
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="28" t="n"/>
       <c r="C42" s="5" t="n"/>
       <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
@@ -2319,6 +2320,11 @@
     <filterColumn colId="4" showButton="0"/>
   </autoFilter>
   <mergeCells count="16">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="B35:B42"/>
     <mergeCell ref="A25:A32"/>
@@ -2330,11 +2336,6 @@
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2384,20 +2385,20 @@
       <c r="F1" s="3" t="n"/>
     </row>
     <row r="2" ht="21" customHeight="1" thickBot="1">
-      <c r="A2" s="37" t="inlineStr">
+      <c r="A2" s="31" t="inlineStr">
         <is>
           <t>اولا : نسبة التالف على الماكينات</t>
         </is>
       </c>
-      <c r="B2" s="28" t="n"/>
-      <c r="C2" s="23" t="inlineStr">
+      <c r="B2" s="32" t="n"/>
+      <c r="C2" s="36" t="inlineStr">
         <is>
           <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
         </is>
       </c>
-      <c r="D2" s="24" t="n"/>
-      <c r="E2" s="24" t="n"/>
-      <c r="F2" s="24" t="n"/>
+      <c r="D2" s="37" t="n"/>
+      <c r="E2" s="37" t="n"/>
+      <c r="F2" s="37" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1" thickBot="1">
       <c r="A3" s="11" t="inlineStr">
@@ -2432,10 +2433,10 @@
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="38" t="n">
+      <c r="A4" s="34" t="n">
         <v>0.5245319561007101</v>
       </c>
-      <c r="B4" s="39" t="n">
+      <c r="B4" s="35" t="n">
         <v>0.4118416589951063</v>
       </c>
       <c r="C4" s="4" t="n">
@@ -2450,8 +2451,8 @@
       <c r="F4" s="9" t="n"/>
     </row>
     <row r="5" ht="21.75" customHeight="1">
-      <c r="A5" s="30" t="n"/>
-      <c r="B5" s="33" t="n"/>
+      <c r="A5" s="24" t="n"/>
+      <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
         <v>30</v>
       </c>
@@ -2528,20 +2529,20 @@
       <c r="F11" s="9" t="n"/>
     </row>
     <row r="12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A12" s="27" t="inlineStr">
+      <c r="A12" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
         </is>
       </c>
-      <c r="B12" s="28" t="n"/>
-      <c r="C12" s="25" t="inlineStr">
+      <c r="B12" s="32" t="n"/>
+      <c r="C12" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D12" s="26" t="n"/>
-      <c r="E12" s="26" t="n"/>
-      <c r="F12" s="26" t="n"/>
+      <c r="D12" s="39" t="n"/>
+      <c r="E12" s="39" t="n"/>
+      <c r="F12" s="39" t="n"/>
     </row>
     <row r="13" ht="18" customHeight="1" thickBot="1">
       <c r="A13" s="11" t="inlineStr">
@@ -2576,10 +2577,10 @@
       </c>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="A14" s="35" t="n">
+      <c r="A14" s="29" t="n">
         <v>7</v>
       </c>
-      <c r="B14" s="36" t="n">
+      <c r="B14" s="30" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="4" t="n">
@@ -2594,8 +2595,8 @@
       <c r="F14" s="9" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
-      <c r="A15" s="30" t="n"/>
-      <c r="B15" s="33" t="n"/>
+      <c r="A15" s="24" t="n"/>
+      <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
         <v>6</v>
       </c>
@@ -2608,48 +2609,48 @@
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
-      <c r="A16" s="30" t="n"/>
-      <c r="B16" s="33" t="n"/>
+      <c r="A16" s="24" t="n"/>
+      <c r="B16" s="27" t="n"/>
       <c r="C16" s="4" t="n"/>
       <c r="D16" s="18" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
-      <c r="A17" s="30" t="n"/>
-      <c r="B17" s="33" t="n"/>
+      <c r="A17" s="24" t="n"/>
+      <c r="B17" s="27" t="n"/>
       <c r="C17" s="4" t="n"/>
       <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="30" t="n"/>
-      <c r="B18" s="33" t="n"/>
+      <c r="A18" s="24" t="n"/>
+      <c r="B18" s="27" t="n"/>
       <c r="C18" s="4" t="n"/>
       <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="30" t="n"/>
-      <c r="B19" s="33" t="n"/>
+      <c r="A19" s="24" t="n"/>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
     <row r="20" ht="18" customHeight="1">
-      <c r="A20" s="30" t="n"/>
-      <c r="B20" s="33" t="n"/>
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="27" t="n"/>
       <c r="C20" s="4" t="n"/>
       <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
     <row r="21" ht="18" customHeight="1">
-      <c r="A21" s="30" t="n"/>
-      <c r="B21" s="33" t="n"/>
+      <c r="A21" s="24" t="n"/>
+      <c r="B21" s="27" t="n"/>
       <c r="C21" s="4" t="n"/>
       <c r="D21" s="18" t="n"/>
       <c r="E21" s="9" t="n"/>
@@ -2664,20 +2665,20 @@
       <c r="F22" s="9" t="n"/>
     </row>
     <row r="23" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A23" s="27" t="inlineStr">
+      <c r="A23" s="33" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
         </is>
       </c>
-      <c r="B23" s="28" t="n"/>
-      <c r="C23" s="25" t="inlineStr">
+      <c r="B23" s="32" t="n"/>
+      <c r="C23" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D23" s="26" t="n"/>
-      <c r="E23" s="26" t="n"/>
-      <c r="F23" s="26" t="n"/>
+      <c r="D23" s="39" t="n"/>
+      <c r="E23" s="39" t="n"/>
+      <c r="F23" s="39" t="n"/>
     </row>
     <row r="24" ht="18" customHeight="1" thickBot="1">
       <c r="A24" s="11" t="inlineStr">
@@ -2712,85 +2713,85 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="35" t="n">
+      <c r="A25" s="29" t="n">
         <v>6</v>
       </c>
-      <c r="B25" s="36" t="n"/>
+      <c r="B25" s="30" t="n"/>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
     <row r="26" ht="18" customHeight="1">
-      <c r="A26" s="30" t="n"/>
-      <c r="B26" s="33" t="n"/>
+      <c r="A26" s="24" t="n"/>
+      <c r="B26" s="27" t="n"/>
       <c r="C26" s="4" t="n"/>
       <c r="D26" s="18" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
     <row r="27" ht="18" customHeight="1">
-      <c r="A27" s="30" t="n"/>
-      <c r="B27" s="33" t="n"/>
+      <c r="A27" s="24" t="n"/>
+      <c r="B27" s="27" t="n"/>
       <c r="C27" s="4" t="n"/>
       <c r="D27" s="18" t="n"/>
       <c r="E27" s="9" t="n"/>
       <c r="F27" s="9" t="n"/>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="A28" s="30" t="n"/>
-      <c r="B28" s="33" t="n"/>
+      <c r="A28" s="24" t="n"/>
+      <c r="B28" s="27" t="n"/>
       <c r="C28" s="4" t="n"/>
       <c r="D28" s="18" t="n"/>
       <c r="E28" s="9" t="n"/>
       <c r="F28" s="9" t="n"/>
     </row>
     <row r="29" ht="18" customHeight="1">
-      <c r="A29" s="30" t="n"/>
-      <c r="B29" s="33" t="n"/>
+      <c r="A29" s="24" t="n"/>
+      <c r="B29" s="27" t="n"/>
       <c r="C29" s="4" t="n"/>
       <c r="D29" s="18" t="n"/>
       <c r="E29" s="9" t="n"/>
       <c r="F29" s="9" t="n"/>
     </row>
     <row r="30" ht="18" customHeight="1">
-      <c r="A30" s="30" t="n"/>
-      <c r="B30" s="33" t="n"/>
+      <c r="A30" s="24" t="n"/>
+      <c r="B30" s="27" t="n"/>
       <c r="C30" s="4" t="n"/>
       <c r="D30" s="18" t="n"/>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="9" t="n"/>
     </row>
     <row r="31" ht="18" customHeight="1">
-      <c r="A31" s="30" t="n"/>
-      <c r="B31" s="33" t="n"/>
+      <c r="A31" s="24" t="n"/>
+      <c r="B31" s="27" t="n"/>
       <c r="C31" s="4" t="n"/>
       <c r="D31" s="18" t="n"/>
       <c r="E31" s="9" t="n"/>
       <c r="F31" s="9" t="n"/>
     </row>
     <row r="32" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A32" s="30" t="n"/>
-      <c r="B32" s="33" t="n"/>
+      <c r="A32" s="24" t="n"/>
+      <c r="B32" s="27" t="n"/>
       <c r="C32" s="5" t="n"/>
       <c r="D32" s="19" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
     </row>
     <row r="33" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A33" s="27" t="inlineStr">
+      <c r="A33" s="33" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
         </is>
       </c>
-      <c r="B33" s="28" t="n"/>
-      <c r="C33" s="25" t="inlineStr">
+      <c r="B33" s="32" t="n"/>
+      <c r="C33" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D33" s="26" t="n"/>
-      <c r="E33" s="26" t="n"/>
+      <c r="D33" s="39" t="n"/>
+      <c r="E33" s="39" t="n"/>
     </row>
     <row r="34" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="11" t="inlineStr">
@@ -2825,10 +2826,10 @@
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" s="29" t="n">
+      <c r="A35" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="B35" s="32" t="n">
+      <c r="B35" s="26" t="n">
         <v>3</v>
       </c>
       <c r="C35" s="4" t="n">
@@ -2843,8 +2844,8 @@
       <c r="F35" s="9" t="n"/>
     </row>
     <row r="36" ht="18" customHeight="1">
-      <c r="A36" s="30" t="n"/>
-      <c r="B36" s="33" t="n"/>
+      <c r="A36" s="24" t="n"/>
+      <c r="B36" s="27" t="n"/>
       <c r="C36" s="4" t="n">
         <v>9</v>
       </c>
@@ -2857,8 +2858,8 @@
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
-      <c r="A37" s="30" t="n"/>
-      <c r="B37" s="33" t="n"/>
+      <c r="A37" s="24" t="n"/>
+      <c r="B37" s="27" t="n"/>
       <c r="C37" s="4" t="n">
         <v>26</v>
       </c>
@@ -2871,40 +2872,40 @@
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1">
-      <c r="A38" s="30" t="n"/>
-      <c r="B38" s="33" t="n"/>
+      <c r="A38" s="24" t="n"/>
+      <c r="B38" s="27" t="n"/>
       <c r="C38" s="4" t="n"/>
       <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
     <row r="39" ht="18" customHeight="1">
-      <c r="A39" s="30" t="n"/>
-      <c r="B39" s="33" t="n"/>
+      <c r="A39" s="24" t="n"/>
+      <c r="B39" s="27" t="n"/>
       <c r="C39" s="4" t="n"/>
       <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
     <row r="40" ht="18" customHeight="1">
-      <c r="A40" s="30" t="n"/>
-      <c r="B40" s="33" t="n"/>
+      <c r="A40" s="24" t="n"/>
+      <c r="B40" s="27" t="n"/>
       <c r="C40" s="4" t="n"/>
       <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="A41" s="30" t="n"/>
-      <c r="B41" s="33" t="n"/>
+      <c r="A41" s="24" t="n"/>
+      <c r="B41" s="27" t="n"/>
       <c r="C41" s="4" t="n"/>
       <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
     <row r="42" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A42" s="31" t="n"/>
-      <c r="B42" s="34" t="n"/>
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="28" t="n"/>
       <c r="C42" s="5" t="n"/>
       <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
@@ -2912,6 +2913,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="B35:B42"/>
     <mergeCell ref="A25:A32"/>
@@ -2923,11 +2929,6 @@
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2942,7 +2943,7 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
@@ -2977,20 +2978,20 @@
       <c r="F1" s="3" t="n"/>
     </row>
     <row r="2" ht="21" customHeight="1" thickBot="1">
-      <c r="A2" s="37" t="inlineStr">
+      <c r="A2" s="31" t="inlineStr">
         <is>
           <t>اولا : نسبة التالف على الماكينات</t>
         </is>
       </c>
-      <c r="B2" s="28" t="n"/>
-      <c r="C2" s="23" t="inlineStr">
+      <c r="B2" s="32" t="n"/>
+      <c r="C2" s="36" t="inlineStr">
         <is>
           <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
         </is>
       </c>
-      <c r="D2" s="24" t="n"/>
-      <c r="E2" s="24" t="n"/>
-      <c r="F2" s="24" t="n"/>
+      <c r="D2" s="37" t="n"/>
+      <c r="E2" s="37" t="n"/>
+      <c r="F2" s="37" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1" thickBot="1">
       <c r="A3" s="11" t="inlineStr">
@@ -3025,10 +3026,10 @@
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="38" t="n">
+      <c r="A4" s="34" t="n">
         <v>0.712523979172376</v>
       </c>
-      <c r="B4" s="39" t="n">
+      <c r="B4" s="35" t="n">
         <v>0.828438017773761</v>
       </c>
       <c r="C4" s="4" t="n">
@@ -3043,8 +3044,8 @@
       <c r="F4" s="9" t="n"/>
     </row>
     <row r="5" ht="21.75" customHeight="1">
-      <c r="A5" s="30" t="n"/>
-      <c r="B5" s="33" t="n"/>
+      <c r="A5" s="24" t="n"/>
+      <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
         <v>4</v>
       </c>
@@ -3127,20 +3128,20 @@
       <c r="F11" s="9" t="n"/>
     </row>
     <row r="12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A12" s="27" t="inlineStr">
+      <c r="A12" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
         </is>
       </c>
-      <c r="B12" s="28" t="n"/>
-      <c r="C12" s="25" t="inlineStr">
+      <c r="B12" s="32" t="n"/>
+      <c r="C12" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D12" s="26" t="n"/>
-      <c r="E12" s="26" t="n"/>
-      <c r="F12" s="26" t="n"/>
+      <c r="D12" s="39" t="n"/>
+      <c r="E12" s="39" t="n"/>
+      <c r="F12" s="39" t="n"/>
     </row>
     <row r="13" ht="18" customHeight="1" thickBot="1">
       <c r="A13" s="11" t="inlineStr">
@@ -3175,10 +3176,10 @@
       </c>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="A14" s="35" t="n">
+      <c r="A14" s="29" t="n">
         <v>7</v>
       </c>
-      <c r="B14" s="36" t="n">
+      <c r="B14" s="30" t="n">
         <v>3</v>
       </c>
       <c r="C14" s="4" t="n">
@@ -3193,8 +3194,8 @@
       <c r="F14" s="9" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
-      <c r="A15" s="30" t="n"/>
-      <c r="B15" s="33" t="n"/>
+      <c r="A15" s="24" t="n"/>
+      <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
         <v>6</v>
       </c>
@@ -3207,8 +3208,8 @@
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
-      <c r="A16" s="30" t="n"/>
-      <c r="B16" s="33" t="n"/>
+      <c r="A16" s="24" t="n"/>
+      <c r="B16" s="27" t="n"/>
       <c r="C16" s="4" t="n">
         <v>7</v>
       </c>
@@ -3221,40 +3222,40 @@
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
-      <c r="A17" s="30" t="n"/>
-      <c r="B17" s="33" t="n"/>
+      <c r="A17" s="24" t="n"/>
+      <c r="B17" s="27" t="n"/>
       <c r="C17" s="4" t="n"/>
       <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="30" t="n"/>
-      <c r="B18" s="33" t="n"/>
+      <c r="A18" s="24" t="n"/>
+      <c r="B18" s="27" t="n"/>
       <c r="C18" s="4" t="n"/>
       <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="30" t="n"/>
-      <c r="B19" s="33" t="n"/>
+      <c r="A19" s="24" t="n"/>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
     <row r="20" ht="18" customHeight="1">
-      <c r="A20" s="30" t="n"/>
-      <c r="B20" s="33" t="n"/>
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="27" t="n"/>
       <c r="C20" s="4" t="n"/>
       <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
     <row r="21" ht="18" customHeight="1">
-      <c r="A21" s="30" t="n"/>
-      <c r="B21" s="33" t="n"/>
+      <c r="A21" s="24" t="n"/>
+      <c r="B21" s="27" t="n"/>
       <c r="C21" s="4" t="n"/>
       <c r="D21" s="18" t="n"/>
       <c r="E21" s="9" t="n"/>
@@ -3269,20 +3270,20 @@
       <c r="F22" s="9" t="n"/>
     </row>
     <row r="23" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A23" s="27" t="inlineStr">
+      <c r="A23" s="33" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
         </is>
       </c>
-      <c r="B23" s="28" t="n"/>
-      <c r="C23" s="25" t="inlineStr">
+      <c r="B23" s="32" t="n"/>
+      <c r="C23" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D23" s="26" t="n"/>
-      <c r="E23" s="26" t="n"/>
-      <c r="F23" s="26" t="n"/>
+      <c r="D23" s="39" t="n"/>
+      <c r="E23" s="39" t="n"/>
+      <c r="F23" s="39" t="n"/>
     </row>
     <row r="24" ht="18" customHeight="1" thickBot="1">
       <c r="A24" s="11" t="inlineStr">
@@ -3317,10 +3318,10 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="35" t="n">
+      <c r="A25" s="29" t="n">
         <v>6</v>
       </c>
-      <c r="B25" s="36" t="n"/>
+      <c r="B25" s="30" t="n"/>
       <c r="C25" s="4" t="n">
         <v>48</v>
       </c>
@@ -3333,75 +3334,75 @@
       <c r="F25" s="9" t="n"/>
     </row>
     <row r="26" ht="18" customHeight="1">
-      <c r="A26" s="30" t="n"/>
-      <c r="B26" s="33" t="n"/>
+      <c r="A26" s="24" t="n"/>
+      <c r="B26" s="27" t="n"/>
       <c r="C26" s="4" t="n"/>
       <c r="D26" s="18" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
     <row r="27" ht="18" customHeight="1">
-      <c r="A27" s="30" t="n"/>
-      <c r="B27" s="33" t="n"/>
+      <c r="A27" s="24" t="n"/>
+      <c r="B27" s="27" t="n"/>
       <c r="C27" s="4" t="n"/>
       <c r="D27" s="18" t="n"/>
       <c r="E27" s="9" t="n"/>
       <c r="F27" s="9" t="n"/>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="A28" s="30" t="n"/>
-      <c r="B28" s="33" t="n"/>
+      <c r="A28" s="24" t="n"/>
+      <c r="B28" s="27" t="n"/>
       <c r="C28" s="4" t="n"/>
       <c r="D28" s="18" t="n"/>
       <c r="E28" s="9" t="n"/>
       <c r="F28" s="9" t="n"/>
     </row>
     <row r="29" ht="18" customHeight="1">
-      <c r="A29" s="30" t="n"/>
-      <c r="B29" s="33" t="n"/>
+      <c r="A29" s="24" t="n"/>
+      <c r="B29" s="27" t="n"/>
       <c r="C29" s="4" t="n"/>
       <c r="D29" s="18" t="n"/>
       <c r="E29" s="9" t="n"/>
       <c r="F29" s="9" t="n"/>
     </row>
     <row r="30" ht="18" customHeight="1">
-      <c r="A30" s="30" t="n"/>
-      <c r="B30" s="33" t="n"/>
+      <c r="A30" s="24" t="n"/>
+      <c r="B30" s="27" t="n"/>
       <c r="C30" s="4" t="n"/>
       <c r="D30" s="18" t="n"/>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="9" t="n"/>
     </row>
     <row r="31" ht="18" customHeight="1">
-      <c r="A31" s="30" t="n"/>
-      <c r="B31" s="33" t="n"/>
+      <c r="A31" s="24" t="n"/>
+      <c r="B31" s="27" t="n"/>
       <c r="C31" s="4" t="n"/>
       <c r="D31" s="18" t="n"/>
       <c r="E31" s="9" t="n"/>
       <c r="F31" s="9" t="n"/>
     </row>
     <row r="32" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A32" s="30" t="n"/>
-      <c r="B32" s="33" t="n"/>
+      <c r="A32" s="24" t="n"/>
+      <c r="B32" s="27" t="n"/>
       <c r="C32" s="5" t="n"/>
       <c r="D32" s="19" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
     </row>
     <row r="33" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A33" s="27" t="inlineStr">
+      <c r="A33" s="33" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
         </is>
       </c>
-      <c r="B33" s="28" t="n"/>
-      <c r="C33" s="25" t="inlineStr">
+      <c r="B33" s="32" t="n"/>
+      <c r="C33" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D33" s="26" t="n"/>
-      <c r="E33" s="26" t="n"/>
+      <c r="D33" s="39" t="n"/>
+      <c r="E33" s="39" t="n"/>
     </row>
     <row r="34" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="11" t="inlineStr">
@@ -3436,10 +3437,10 @@
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" s="29" t="n">
+      <c r="A35" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="B35" s="32" t="n">
+      <c r="B35" s="26" t="n">
         <v>4</v>
       </c>
       <c r="C35" s="4" t="n">
@@ -3454,8 +3455,8 @@
       <c r="F35" s="9" t="n"/>
     </row>
     <row r="36" ht="18" customHeight="1">
-      <c r="A36" s="30" t="n"/>
-      <c r="B36" s="33" t="n"/>
+      <c r="A36" s="24" t="n"/>
+      <c r="B36" s="27" t="n"/>
       <c r="C36" s="4" t="n">
         <v>9</v>
       </c>
@@ -3468,8 +3469,8 @@
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
-      <c r="A37" s="30" t="n"/>
-      <c r="B37" s="33" t="n"/>
+      <c r="A37" s="24" t="n"/>
+      <c r="B37" s="27" t="n"/>
       <c r="C37" s="4" t="n">
         <v>26</v>
       </c>
@@ -3482,40 +3483,40 @@
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1">
-      <c r="A38" s="30" t="n"/>
-      <c r="B38" s="33" t="n"/>
+      <c r="A38" s="24" t="n"/>
+      <c r="B38" s="27" t="n"/>
       <c r="C38" s="4" t="n"/>
       <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
     <row r="39" ht="18" customHeight="1">
-      <c r="A39" s="30" t="n"/>
-      <c r="B39" s="33" t="n"/>
+      <c r="A39" s="24" t="n"/>
+      <c r="B39" s="27" t="n"/>
       <c r="C39" s="4" t="n"/>
       <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
     <row r="40" ht="18" customHeight="1">
-      <c r="A40" s="30" t="n"/>
-      <c r="B40" s="33" t="n"/>
+      <c r="A40" s="24" t="n"/>
+      <c r="B40" s="27" t="n"/>
       <c r="C40" s="4" t="n"/>
       <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="A41" s="30" t="n"/>
-      <c r="B41" s="33" t="n"/>
+      <c r="A41" s="24" t="n"/>
+      <c r="B41" s="27" t="n"/>
       <c r="C41" s="4" t="n"/>
       <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
     <row r="42" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A42" s="31" t="n"/>
-      <c r="B42" s="34" t="n"/>
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="28" t="n"/>
       <c r="C42" s="5" t="n"/>
       <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
@@ -3523,6 +3524,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="B35:B42"/>
     <mergeCell ref="A25:A32"/>
@@ -3534,11 +3540,6 @@
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3546,6 +3547,611 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="26.625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.625" customWidth="1" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="21" min="4" max="4"/>
+    <col width="28.875" customWidth="1" min="5" max="5"/>
+    <col width="31.875" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" thickBot="1">
+      <c r="A2" s="31" t="inlineStr">
+        <is>
+          <t>اولا : نسبة التالف على الماكينات</t>
+        </is>
+      </c>
+      <c r="B2" s="32" t="n"/>
+      <c r="C2" s="36" t="inlineStr">
+        <is>
+          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
+        </is>
+      </c>
+      <c r="D2" s="37" t="n"/>
+      <c r="E2" s="37" t="n"/>
+      <c r="F2" s="37" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A3" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D3" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.75" customHeight="1">
+      <c r="A4" s="34" t="n">
+        <v>0.7400714254980423</v>
+      </c>
+      <c r="B4" s="35" t="n">
+        <v>0.9533839587606008</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+    </row>
+    <row r="5" ht="21.75" customHeight="1">
+      <c r="A5" s="24" t="n"/>
+      <c r="B5" s="27" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+    </row>
+    <row r="6" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B6" s="12" t="inlineStr">
+        <is>
+          <t>اعلي نسبة توالف</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="18" t="n"/>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="21.75" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="15" t="n"/>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="18" t="n"/>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+    </row>
+    <row r="8" ht="21.75" customHeight="1">
+      <c r="A8" s="13" t="n"/>
+      <c r="B8" s="14" t="n"/>
+      <c r="C8" s="4" t="n"/>
+      <c r="D8" s="18" t="n"/>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="inlineStr">
+        <is>
+          <t>وسيط التوالف</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n"/>
+      <c r="D9" s="18" t="n"/>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="15" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="18" t="n"/>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="15" t="n"/>
+      <c r="C11" s="5" t="n"/>
+      <c r="D11" s="19" t="n"/>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A12" s="33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
+        </is>
+      </c>
+      <c r="B12" s="32" t="n"/>
+      <c r="C12" s="38" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D12" s="39" t="n"/>
+      <c r="E12" s="39" t="n"/>
+      <c r="F12" s="39" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="A13" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D13" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="29" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>LG 65UP77 FRONT</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1">
+      <c r="A15" s="24" t="n"/>
+      <c r="B15" s="27" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="9" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="24" t="n"/>
+      <c r="B16" s="27" t="n"/>
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="18" t="n"/>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1">
+      <c r="A17" s="24" t="n"/>
+      <c r="B17" s="27" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="24" t="n"/>
+      <c r="B18" s="27" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="24" t="n"/>
+      <c r="B19" s="27" t="n"/>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="18" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="27" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="18" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="24" t="n"/>
+      <c r="B21" s="27" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="18" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A22" s="22" t="n"/>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="20" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+    </row>
+    <row r="23" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A23" s="33" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
+        </is>
+      </c>
+      <c r="B23" s="32" t="n"/>
+      <c r="C23" s="38" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D23" s="39" t="n"/>
+      <c r="E23" s="39" t="n"/>
+      <c r="F23" s="39" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B24" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D24" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="29" t="n">
+        <v>7</v>
+      </c>
+      <c r="B25" s="30" t="n"/>
+      <c r="C25" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="24" t="n"/>
+      <c r="B26" s="27" t="n"/>
+      <c r="C26" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D26" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1">
+      <c r="A27" s="24" t="n"/>
+      <c r="B27" s="27" t="n"/>
+      <c r="C27" s="4" t="n"/>
+      <c r="D27" s="18" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1">
+      <c r="A28" s="24" t="n"/>
+      <c r="B28" s="27" t="n"/>
+      <c r="C28" s="4" t="n"/>
+      <c r="D28" s="18" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1">
+      <c r="A29" s="24" t="n"/>
+      <c r="B29" s="27" t="n"/>
+      <c r="C29" s="4" t="n"/>
+      <c r="D29" s="18" t="n"/>
+      <c r="E29" s="9" t="n"/>
+      <c r="F29" s="9" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="24" t="n"/>
+      <c r="B30" s="27" t="n"/>
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="18" t="n"/>
+      <c r="E30" s="9" t="n"/>
+      <c r="F30" s="9" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="24" t="n"/>
+      <c r="B31" s="27" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="18" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A32" s="24" t="n"/>
+      <c r="B32" s="27" t="n"/>
+      <c r="C32" s="5" t="n"/>
+      <c r="D32" s="19" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A33" s="33" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
+        </is>
+      </c>
+      <c r="B33" s="32" t="n"/>
+      <c r="C33" s="38" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D33" s="39" t="n"/>
+      <c r="E33" s="39" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1">
+      <c r="A34" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B34" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D34" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1">
+      <c r="A35" s="23" t="n">
+        <v>7</v>
+      </c>
+      <c r="B35" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" s="18" t="inlineStr">
+        <is>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
+        </is>
+      </c>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1">
+      <c r="A36" s="24" t="n"/>
+      <c r="B36" s="27" t="n"/>
+      <c r="C36" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D36" s="18" t="inlineStr">
+        <is>
+          <t>LG 65UP77 FRONT</t>
+        </is>
+      </c>
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="9" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1">
+      <c r="A37" s="24" t="n"/>
+      <c r="B37" s="27" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D37" s="18" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="9" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1">
+      <c r="A38" s="24" t="n"/>
+      <c r="B38" s="27" t="n"/>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="18" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1">
+      <c r="A39" s="24" t="n"/>
+      <c r="B39" s="27" t="n"/>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="18" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1">
+      <c r="A40" s="24" t="n"/>
+      <c r="B40" s="27" t="n"/>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="18" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1">
+      <c r="A41" s="24" t="n"/>
+      <c r="B41" s="27" t="n"/>
+      <c r="C41" s="4" t="n"/>
+      <c r="D41" s="18" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+    </row>
+    <row r="42" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="28" t="n"/>
+      <c r="C42" s="5" t="n"/>
+      <c r="D42" s="19" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="10" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3575,7 +4181,7 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
@@ -3588,20 +4194,20 @@
       <c r="F1" s="3" t="n"/>
     </row>
     <row r="2" ht="21" customHeight="1" thickBot="1">
-      <c r="A2" s="37" t="inlineStr">
+      <c r="A2" s="31" t="inlineStr">
         <is>
           <t>اولا : نسبة التالف على الماكينات</t>
         </is>
       </c>
-      <c r="B2" s="28" t="n"/>
-      <c r="C2" s="23" t="inlineStr">
+      <c r="B2" s="32" t="n"/>
+      <c r="C2" s="36" t="inlineStr">
         <is>
           <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
         </is>
       </c>
-      <c r="D2" s="24" t="n"/>
-      <c r="E2" s="24" t="n"/>
-      <c r="F2" s="24" t="n"/>
+      <c r="D2" s="37" t="n"/>
+      <c r="E2" s="37" t="n"/>
+      <c r="F2" s="37" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1" thickBot="1">
       <c r="A3" s="11" t="inlineStr">
@@ -3636,32 +4242,32 @@
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="38" t="n">
-        <v>0.7400714254980423</v>
-      </c>
-      <c r="B4" s="39" t="n">
-        <v>0.9533839587606008</v>
+      <c r="A4" s="34" t="n">
+        <v>0.5386377131224023</v>
+      </c>
+      <c r="B4" s="35" t="n">
+        <v>0.6558220279045843</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+          <t>فوم طقم رويال جاز المعدل</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
     </row>
     <row r="5" ht="21.75" customHeight="1">
-      <c r="A5" s="30" t="n"/>
-      <c r="B5" s="33" t="n"/>
+      <c r="A5" s="24" t="n"/>
+      <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>LG65UP77_TB</t>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -3678,8 +4284,14 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
@@ -3732,20 +4344,20 @@
       <c r="F11" s="9" t="n"/>
     </row>
     <row r="12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A12" s="27" t="inlineStr">
+      <c r="A12" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
         </is>
       </c>
-      <c r="B12" s="28" t="n"/>
-      <c r="C12" s="25" t="inlineStr">
+      <c r="B12" s="32" t="n"/>
+      <c r="C12" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D12" s="26" t="n"/>
-      <c r="E12" s="26" t="n"/>
-      <c r="F12" s="26" t="n"/>
+      <c r="D12" s="39" t="n"/>
+      <c r="E12" s="39" t="n"/>
+      <c r="F12" s="39" t="n"/>
     </row>
     <row r="13" ht="18" customHeight="1" thickBot="1">
       <c r="A13" s="11" t="inlineStr">
@@ -3780,10 +4392,10 @@
       </c>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="A14" s="35" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="36" t="n">
+      <c r="A14" s="29" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="30" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="4" t="n">
@@ -3798,62 +4410,62 @@
       <c r="F14" s="9" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
-      <c r="A15" s="30" t="n"/>
-      <c r="B15" s="33" t="n"/>
+      <c r="A15" s="24" t="n"/>
+      <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
         <v>7</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
-      <c r="A16" s="30" t="n"/>
-      <c r="B16" s="33" t="n"/>
+      <c r="A16" s="24" t="n"/>
+      <c r="B16" s="27" t="n"/>
       <c r="C16" s="4" t="n"/>
       <c r="D16" s="18" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
-      <c r="A17" s="30" t="n"/>
-      <c r="B17" s="33" t="n"/>
+      <c r="A17" s="24" t="n"/>
+      <c r="B17" s="27" t="n"/>
       <c r="C17" s="4" t="n"/>
       <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="30" t="n"/>
-      <c r="B18" s="33" t="n"/>
+      <c r="A18" s="24" t="n"/>
+      <c r="B18" s="27" t="n"/>
       <c r="C18" s="4" t="n"/>
       <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="30" t="n"/>
-      <c r="B19" s="33" t="n"/>
+      <c r="A19" s="24" t="n"/>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
     <row r="20" ht="18" customHeight="1">
-      <c r="A20" s="30" t="n"/>
-      <c r="B20" s="33" t="n"/>
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="27" t="n"/>
       <c r="C20" s="4" t="n"/>
       <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
     <row r="21" ht="18" customHeight="1">
-      <c r="A21" s="30" t="n"/>
-      <c r="B21" s="33" t="n"/>
+      <c r="A21" s="24" t="n"/>
+      <c r="B21" s="27" t="n"/>
       <c r="C21" s="4" t="n"/>
       <c r="D21" s="18" t="n"/>
       <c r="E21" s="9" t="n"/>
@@ -3868,20 +4480,20 @@
       <c r="F22" s="9" t="n"/>
     </row>
     <row r="23" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A23" s="27" t="inlineStr">
+      <c r="A23" s="33" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
         </is>
       </c>
-      <c r="B23" s="28" t="n"/>
-      <c r="C23" s="25" t="inlineStr">
+      <c r="B23" s="32" t="n"/>
+      <c r="C23" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D23" s="26" t="n"/>
-      <c r="E23" s="26" t="n"/>
-      <c r="F23" s="26" t="n"/>
+      <c r="D23" s="39" t="n"/>
+      <c r="E23" s="39" t="n"/>
+      <c r="F23" s="39" t="n"/>
     </row>
     <row r="24" ht="18" customHeight="1" thickBot="1">
       <c r="A24" s="11" t="inlineStr">
@@ -3916,99 +4528,99 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="35" t="n">
-        <v>7</v>
-      </c>
-      <c r="B25" s="36" t="n">
+      <c r="A25" s="29" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" s="30" t="n">
         <v/>
       </c>
       <c r="C25" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D25" s="18" t="inlineStr">
         <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
+          <t>صندوق سمك 5ك بنى سويف</t>
         </is>
       </c>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
     <row r="26" ht="18" customHeight="1">
-      <c r="A26" s="30" t="n"/>
-      <c r="B26" s="33" t="n"/>
+      <c r="A26" s="24" t="n"/>
+      <c r="B26" s="27" t="n"/>
       <c r="C26" s="4" t="n">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D26" s="18" t="inlineStr">
         <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
         </is>
       </c>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
     <row r="27" ht="18" customHeight="1">
-      <c r="A27" s="30" t="n"/>
-      <c r="B27" s="33" t="n"/>
+      <c r="A27" s="24" t="n"/>
+      <c r="B27" s="27" t="n"/>
       <c r="C27" s="4" t="n"/>
       <c r="D27" s="18" t="n"/>
       <c r="E27" s="9" t="n"/>
       <c r="F27" s="9" t="n"/>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="A28" s="30" t="n"/>
-      <c r="B28" s="33" t="n"/>
+      <c r="A28" s="24" t="n"/>
+      <c r="B28" s="27" t="n"/>
       <c r="C28" s="4" t="n"/>
       <c r="D28" s="18" t="n"/>
       <c r="E28" s="9" t="n"/>
       <c r="F28" s="9" t="n"/>
     </row>
     <row r="29" ht="18" customHeight="1">
-      <c r="A29" s="30" t="n"/>
-      <c r="B29" s="33" t="n"/>
+      <c r="A29" s="24" t="n"/>
+      <c r="B29" s="27" t="n"/>
       <c r="C29" s="4" t="n"/>
       <c r="D29" s="18" t="n"/>
       <c r="E29" s="9" t="n"/>
       <c r="F29" s="9" t="n"/>
     </row>
     <row r="30" ht="18" customHeight="1">
-      <c r="A30" s="30" t="n"/>
-      <c r="B30" s="33" t="n"/>
+      <c r="A30" s="24" t="n"/>
+      <c r="B30" s="27" t="n"/>
       <c r="C30" s="4" t="n"/>
       <c r="D30" s="18" t="n"/>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="9" t="n"/>
     </row>
     <row r="31" ht="18" customHeight="1">
-      <c r="A31" s="30" t="n"/>
-      <c r="B31" s="33" t="n"/>
+      <c r="A31" s="24" t="n"/>
+      <c r="B31" s="27" t="n"/>
       <c r="C31" s="4" t="n"/>
       <c r="D31" s="18" t="n"/>
       <c r="E31" s="9" t="n"/>
       <c r="F31" s="9" t="n"/>
     </row>
     <row r="32" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A32" s="30" t="n"/>
-      <c r="B32" s="33" t="n"/>
+      <c r="A32" s="24" t="n"/>
+      <c r="B32" s="27" t="n"/>
       <c r="C32" s="5" t="n"/>
       <c r="D32" s="19" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
     </row>
     <row r="33" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A33" s="27" t="inlineStr">
+      <c r="A33" s="33" t="inlineStr">
         <is>
           <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
         </is>
       </c>
-      <c r="B33" s="28" t="n"/>
-      <c r="C33" s="25" t="inlineStr">
+      <c r="B33" s="32" t="n"/>
+      <c r="C33" s="38" t="inlineStr">
         <is>
           <t>ملاحظات</t>
         </is>
       </c>
-      <c r="D33" s="26" t="n"/>
-      <c r="E33" s="26" t="n"/>
+      <c r="D33" s="39" t="n"/>
+      <c r="E33" s="39" t="n"/>
     </row>
     <row r="34" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="11" t="inlineStr">
@@ -4043,14 +4655,14 @@
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" s="29" t="n">
-        <v>7</v>
-      </c>
-      <c r="B35" s="32" t="n">
-        <v>5</v>
+      <c r="A35" s="23" t="n">
+        <v>9</v>
+      </c>
+      <c r="B35" s="26" t="n">
+        <v>6</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
@@ -4061,68 +4673,74 @@
       <c r="F35" s="9" t="n"/>
     </row>
     <row r="36" ht="18" customHeight="1">
-      <c r="A36" s="30" t="n"/>
-      <c r="B36" s="33" t="n"/>
+      <c r="A36" s="24" t="n"/>
+      <c r="B36" s="27" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36" s="18" t="inlineStr">
         <is>
-          <t>LG 65UP77 FRONT</t>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
-      <c r="A37" s="30" t="n"/>
-      <c r="B37" s="33" t="n"/>
+      <c r="A37" s="24" t="n"/>
+      <c r="B37" s="27" t="n"/>
       <c r="C37" s="4" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D37" s="18" t="inlineStr">
         <is>
-          <t>LG65UM73</t>
+          <t>كفر غسالة LG/زوايا غسالة LG</t>
         </is>
       </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1">
-      <c r="A38" s="30" t="n"/>
-      <c r="B38" s="33" t="n"/>
-      <c r="C38" s="4" t="n"/>
-      <c r="D38" s="18" t="n"/>
+      <c r="A38" s="24" t="n"/>
+      <c r="B38" s="27" t="n"/>
+      <c r="C38" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="D38" s="18" t="inlineStr">
+        <is>
+          <t>فوم كوش 130</t>
+        </is>
+      </c>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
     <row r="39" ht="18" customHeight="1">
-      <c r="A39" s="30" t="n"/>
-      <c r="B39" s="33" t="n"/>
+      <c r="A39" s="24" t="n"/>
+      <c r="B39" s="27" t="n"/>
       <c r="C39" s="4" t="n"/>
       <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
     <row r="40" ht="18" customHeight="1">
-      <c r="A40" s="30" t="n"/>
-      <c r="B40" s="33" t="n"/>
+      <c r="A40" s="24" t="n"/>
+      <c r="B40" s="27" t="n"/>
       <c r="C40" s="4" t="n"/>
       <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="A41" s="30" t="n"/>
-      <c r="B41" s="33" t="n"/>
+      <c r="A41" s="24" t="n"/>
+      <c r="B41" s="27" t="n"/>
       <c r="C41" s="4" t="n"/>
       <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
     <row r="42" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A42" s="31" t="n"/>
-      <c r="B42" s="34" t="n"/>
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="28" t="n"/>
       <c r="C42" s="5" t="n"/>
       <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
@@ -4130,6 +4748,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="B35:B42"/>
     <mergeCell ref="A25:A32"/>
@@ -4141,11 +4764,6 @@
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>